<commit_message>
Support for first pass formatting checks
</commit_message>
<xml_diff>
--- a/public/examples/iepd-requirements-example.xlsx
+++ b/public/examples/iepd-requirements-example.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\cdmgtri\niem-mapping\examples\iepd-requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\cdmgtri\niem-mapping-app\public\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10548" yWindow="1620" windowWidth="19440" windowHeight="11676" tabRatio="890" activeTab="9"/>
+    <workbookView xWindow="10548" yWindow="1620" windowWidth="19440" windowHeight="11676" tabRatio="890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" r:id="rId1"/>
@@ -30,9 +30,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$N$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
-    <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$132:$B$141</definedName>
-    <definedName name="CODES_NDRArtifact">'Field Descriptions'!$B$148:$B$149</definedName>
-    <definedName name="CODES_NDRVersion">'Field Descriptions'!$B$145:$B$146</definedName>
+    <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$164:$B$173</definedName>
+    <definedName name="CODES_NDRArtifact">'Field Descriptions'!$B$180:$B$181</definedName>
+    <definedName name="CODES_NDRVersion">'Field Descriptions'!$B$177:$B$178</definedName>
     <definedName name="Facet_Mapping_Code">'Codes | Facets'!$F$1</definedName>
     <definedName name="Facet_Mapping_Description">'Codes | Facets'!$G$1</definedName>
     <definedName name="Facet_Mapping_Notes">'Codes | Facets'!$H$1</definedName>
@@ -62,9 +62,10 @@
     <definedName name="HasA_Target_Property_NamespacePrefix">'Type-Has-Property'!$L$1</definedName>
     <definedName name="HasA_Target_Type_Name">'Type-Has-Property'!$K$1</definedName>
     <definedName name="HasA_Target_Type_NamespacePrefix">'Type-Has-Property'!$J$1</definedName>
-    <definedName name="Info_Mapping_Contact">Info!$B$16</definedName>
-    <definedName name="Info_Mapping_Description">Info!$B$14</definedName>
-    <definedName name="Info_Mapping_Status">Info!$B$15</definedName>
+    <definedName name="Info_Mapping_Artifact">Info!$B$14</definedName>
+    <definedName name="Info_Mapping_Contact">Info!$B$17</definedName>
+    <definedName name="Info_Mapping_Description">Info!$B$15</definedName>
+    <definedName name="Info_Mapping_Status">Info!$B$16</definedName>
     <definedName name="Info_Mapping_Summary">Info!$B$13</definedName>
     <definedName name="Info_Source_Contact">Info!$B$9</definedName>
     <definedName name="Info_Source_Date">Info!$B$5</definedName>
@@ -73,14 +74,15 @@
     <definedName name="Info_Source_URL">Info!$B$8</definedName>
     <definedName name="Info_Source_Version">Info!$B$4</definedName>
     <definedName name="Info_Source_Website">Info!$B$7</definedName>
-    <definedName name="Info_Target_Contact">Info!$B$25</definedName>
-    <definedName name="Info_Target_Description">Info!$B$21</definedName>
-    <definedName name="Info_Target_Name">Info!$B$20</definedName>
-    <definedName name="Info_Target_NIEMRelease">Info!$B$22</definedName>
-    <definedName name="Info_Target_URL">Info!$B$24</definedName>
-    <definedName name="Info_Target_Website">Info!$B$23</definedName>
-    <definedName name="MAPPING_CODES">Readme!$A$18:$A$25</definedName>
-    <definedName name="MAPPING_CODES_EXTENDED">Readme!$A$18:$A$26</definedName>
+    <definedName name="Info_Target_Contact">Info!$B$26</definedName>
+    <definedName name="Info_Target_Description">Info!$B$22</definedName>
+    <definedName name="Info_Target_Name">Info!$B$21</definedName>
+    <definedName name="Info_Target_NIEMRelease">Info!$B$23</definedName>
+    <definedName name="Info_Target_URL">Info!$B$25</definedName>
+    <definedName name="Info_Target_Website">Info!$B$24</definedName>
+    <definedName name="MAPPING_ARTIFACTS">'Field Descriptions'!$B$15:$B$22</definedName>
+    <definedName name="MAPPING_CODES">Readme!$A$18:$A$26</definedName>
+    <definedName name="MAPPING_CODES_EXTENDED">Readme!$A$18:$A$27</definedName>
     <definedName name="Namespace_Mapping_Code">Namespace!$D$1</definedName>
     <definedName name="Namespace_Mapping_Description">Namespace!$E$1</definedName>
     <definedName name="Namespace_Mapping_Notes">Namespace!$F$1</definedName>
@@ -124,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="641">
   <si>
     <t>Definition</t>
   </si>
@@ -2265,9 +2267,6 @@
     <t>A data type for a duration of time with the format PnYnMnDTnHnMnS, where nY is the number of years, nM is the number of months, nD is the number of days, nH is the number of hours, nM is the number of minutes, and nS is the number of seconds.</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>Document the lack of a suitable mapping between a source standard and a target standard.</t>
   </si>
   <si>
@@ -3246,12 +3245,158 @@
       <t>1</t>
     </r>
   </si>
+  <si>
+    <t>Info Tab</t>
+  </si>
+  <si>
+    <t>Artifact (*)</t>
+  </si>
+  <si>
+    <t>Source information</t>
+  </si>
+  <si>
+    <t>Target information</t>
+  </si>
+  <si>
+    <t>map standard</t>
+  </si>
+  <si>
+    <t>map IEPD requirements</t>
+  </si>
+  <si>
+    <t>change request</t>
+  </si>
+  <si>
+    <t>map sources</t>
+  </si>
+  <si>
+    <t>documentation</t>
+  </si>
+  <si>
+    <t>change log</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>translation</t>
+  </si>
+  <si>
+    <t>Document a NIEM component.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">REQUIRED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Document the NIEM components.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N/A:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use the "map" code instead to document source info.</t>
+    </r>
+  </si>
+  <si>
+    <t>Map a standard to NIEM.</t>
+  </si>
+  <si>
+    <t>Map local exchange requirements to NIEM components and extensions in the process of building or documenting an IEPD.</t>
+  </si>
+  <si>
+    <t>Map the original source(s) for NIEM components.</t>
+  </si>
+  <si>
+    <t>Source name.</t>
+  </si>
+  <si>
+    <t>Source version.</t>
+  </si>
+  <si>
+    <t>Source date.</t>
+  </si>
+  <si>
+    <t>Description of the source.</t>
+  </si>
+  <si>
+    <t>Informational website for the source.</t>
+  </si>
+  <si>
+    <t>URL for schemas or other kinds of technical documentation or artifacts for the source components.</t>
+  </si>
+  <si>
+    <t>Contact information for the source.</t>
+  </si>
+  <si>
+    <t>A summary or purpose for the mapping.</t>
+  </si>
+  <si>
+    <t>Document proposed modifications to NIEM content for a future release.  This is one of the accepted formats for NIEM content changes.</t>
+  </si>
+  <si>
+    <t>Document NIEM components.</t>
+  </si>
+  <si>
+    <t>Map changes to components between two NIEM releases.</t>
+  </si>
+  <si>
+    <t>Translate NIEM component names and definitions into another language.</t>
+  </si>
+  <si>
+    <t>Additional information about the mapping.</t>
+  </si>
+  <si>
+    <t>Status information about the mapping.</t>
+  </si>
+  <si>
+    <t>Contact information for the person or organization who did the mapping.</t>
+  </si>
+  <si>
+    <t>Target name, e.g., NIEM 4.1, Acme IEPD</t>
+  </si>
+  <si>
+    <t>A description of the target.</t>
+  </si>
+  <si>
+    <t>The NIEM release on which the target is based.  To be used when the target is an IEPD or other artifact that uses NIEM, and not a NIEM release itself.</t>
+  </si>
+  <si>
+    <t>Informational website for the target.</t>
+  </si>
+  <si>
+    <t>URL for schemas or other kinds of technical documentation or artifacts for the target components.</t>
+  </si>
+  <si>
+    <t>Contact information for the target.</t>
+  </si>
+  <si>
+    <t>no match</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3421,6 +3566,12 @@
       <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3604,7 +3755,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3828,6 +3979,19 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -3940,12 +4104,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -4015,6 +4173,12 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4855,64 +5019,64 @@
   <autoFilter ref="A1:K2"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Source_x000a_NS Prefix" dataDxfId="36"/>
-    <tableColumn id="10" name="Term 1" dataDxfId="1"/>
-    <tableColumn id="2" name="Literal 1" dataDxfId="35"/>
-    <tableColumn id="3" name="Definition 1" dataDxfId="34"/>
-    <tableColumn id="4" name="Mapping_x000a_Code" dataDxfId="33"/>
-    <tableColumn id="5" name="Description" dataDxfId="32"/>
-    <tableColumn id="6" name="Notes" dataDxfId="31"/>
-    <tableColumn id="7" name="Target_x000a_NS Prefix" dataDxfId="30"/>
-    <tableColumn id="11" name="Term 2" dataDxfId="0"/>
-    <tableColumn id="8" name="Literal 2" dataDxfId="29"/>
-    <tableColumn id="9" name="Definition 2" dataDxfId="28"/>
+    <tableColumn id="10" name="Term 1" dataDxfId="35"/>
+    <tableColumn id="2" name="Literal 1" dataDxfId="34"/>
+    <tableColumn id="3" name="Definition 1" dataDxfId="33"/>
+    <tableColumn id="4" name="Mapping_x000a_Code" dataDxfId="32"/>
+    <tableColumn id="5" name="Description" dataDxfId="31"/>
+    <tableColumn id="6" name="Notes" dataDxfId="30"/>
+    <tableColumn id="7" name="Target_x000a_NS Prefix" dataDxfId="29"/>
+    <tableColumn id="11" name="Term 2" dataDxfId="28"/>
+    <tableColumn id="8" name="Literal 2" dataDxfId="27"/>
+    <tableColumn id="9" name="Definition 2" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:K3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:K3" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K3"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Source_x000a_Union NS" dataDxfId="25"/>
-    <tableColumn id="2" name="Union Type Name 1" dataDxfId="24"/>
-    <tableColumn id="3" name="Member NS 1" dataDxfId="23"/>
-    <tableColumn id="4" name="Member Type Name 1" dataDxfId="22"/>
-    <tableColumn id="5" name="Mapping_x000a_Code" dataDxfId="21"/>
-    <tableColumn id="6" name="Description" dataDxfId="20"/>
-    <tableColumn id="7" name="Notes" dataDxfId="19"/>
-    <tableColumn id="8" name="Target_x000a_Union NS" dataDxfId="18"/>
-    <tableColumn id="9" name="Union Type Name 2" dataDxfId="17"/>
-    <tableColumn id="10" name="Member NS 2" dataDxfId="16"/>
-    <tableColumn id="11" name="Member Type Name 2" dataDxfId="15"/>
+    <tableColumn id="1" name="Source_x000a_Union NS" dataDxfId="23"/>
+    <tableColumn id="2" name="Union Type Name 1" dataDxfId="22"/>
+    <tableColumn id="3" name="Member NS 1" dataDxfId="21"/>
+    <tableColumn id="4" name="Member Type Name 1" dataDxfId="20"/>
+    <tableColumn id="5" name="Mapping_x000a_Code" dataDxfId="19"/>
+    <tableColumn id="6" name="Description" dataDxfId="18"/>
+    <tableColumn id="7" name="Notes" dataDxfId="17"/>
+    <tableColumn id="8" name="Target_x000a_Union NS" dataDxfId="16"/>
+    <tableColumn id="9" name="Union Type Name 2" dataDxfId="15"/>
+    <tableColumn id="10" name="Member NS 2" dataDxfId="14"/>
+    <tableColumn id="11" name="Member Type Name 2" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1210" displayName="Table1210" ref="A1:K3" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1210" displayName="Table1210" ref="A1:K3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K3"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Source_x000a_Metadata NS" dataDxfId="12"/>
-    <tableColumn id="2" name="Metadata Type Name 1" dataDxfId="11"/>
-    <tableColumn id="3" name="Applies to NS 1" dataDxfId="10"/>
-    <tableColumn id="4" name="Applies to Type Name 1" dataDxfId="9"/>
-    <tableColumn id="5" name="Mapping_x000a_Code" dataDxfId="8"/>
-    <tableColumn id="6" name="Description" dataDxfId="7"/>
-    <tableColumn id="7" name="Notes" dataDxfId="6"/>
-    <tableColumn id="8" name="Target_x000a_Metadata NS 2" dataDxfId="5"/>
-    <tableColumn id="9" name="Metadata Type Name 2" dataDxfId="4"/>
-    <tableColumn id="10" name="Applies to NS 2" dataDxfId="3"/>
-    <tableColumn id="11" name="Applies to Type Name 2" dataDxfId="2"/>
+    <tableColumn id="1" name="Source_x000a_Metadata NS" dataDxfId="10"/>
+    <tableColumn id="2" name="Metadata Type Name 1" dataDxfId="9"/>
+    <tableColumn id="3" name="Applies to NS 1" dataDxfId="8"/>
+    <tableColumn id="4" name="Applies to Type Name 1" dataDxfId="7"/>
+    <tableColumn id="5" name="Mapping_x000a_Code" dataDxfId="6"/>
+    <tableColumn id="6" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" name="Notes" dataDxfId="4"/>
+    <tableColumn id="8" name="Target_x000a_Metadata NS 2" dataDxfId="3"/>
+    <tableColumn id="9" name="Metadata Type Name 2" dataDxfId="2"/>
+    <tableColumn id="10" name="Applies to NS 2" dataDxfId="1"/>
+    <tableColumn id="11" name="Applies to Type Name 2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A29:B38" totalsRowShown="0" headerRowDxfId="132" dataDxfId="131" tableBorderDxfId="130" headerRowCellStyle="Neutral">
-  <autoFilter ref="A29:B38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A30:B39" totalsRowShown="0" headerRowDxfId="132" dataDxfId="131" tableBorderDxfId="130" headerRowCellStyle="Neutral">
+  <autoFilter ref="A30:B39"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Tips and tricks" dataDxfId="129"/>
     <tableColumn id="2" name="Description" dataDxfId="128"/>
@@ -4932,7 +5096,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A12:B16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A12:B17" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="MAPPING INFORMATION" dataDxfId="125"/>
     <tableColumn id="2" name=" " dataDxfId="124"/>
@@ -4942,7 +5106,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A19:B25" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A20:B26" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="TARGET INFORMATION" dataDxfId="123"/>
     <tableColumn id="2" name=" " dataDxfId="122"/>
@@ -5332,7 +5496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5593,7 +5757,7 @@
         <v>88</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>72</v>
@@ -5601,16 +5765,16 @@
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="B24" s="39" t="s">
         <v>533</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="C24" s="31" t="s">
         <v>534</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="D24" s="31" t="s">
         <v>535</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5627,98 +5791,112 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
+        <v>609</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>613</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>615</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B27" s="39" t="s">
         <v>242</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D27" s="31" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="35" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B30" s="35" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+    <row r="31" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+    <row r="33" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+    <row r="34" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+    <row r="35" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="51" t="s">
+    <row r="38" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="51" t="s">
+        <v>539</v>
+      </c>
+      <c r="B38" s="51" t="s">
         <v>540</v>
       </c>
-      <c r="B37" s="51" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A38" s="51" t="s">
+    </row>
+    <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A39" s="51" t="s">
+        <v>546</v>
+      </c>
+      <c r="B39" s="51" t="s">
         <v>547</v>
-      </c>
-      <c r="B38" s="51" t="s">
-        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -5735,9 +5913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5760,13 +5938,13 @@
         <v>245</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>589</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>591</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>49</v>
@@ -5781,13 +5959,13 @@
         <v>247</v>
       </c>
       <c r="I1" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>592</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>593</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -5810,7 +5988,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5830,16 +6008,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>586</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>587</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="3" t="s">
         <v>588</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>589</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>49</v>
@@ -5851,16 +6029,16 @@
         <v>23</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>583</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>584</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>585</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>586</v>
       </c>
     </row>
   </sheetData>
@@ -5879,7 +6057,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C188"/>
+  <dimension ref="A3:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5892,797 +6070,803 @@
     <col min="6" max="16384" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
+      <c r="A3" s="84" t="s">
+        <v>601</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
-        <v>132</v>
+        <v>603</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="38" t="s">
+      <c r="A5" s="85"/>
+      <c r="B5" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="85"/>
+      <c r="B6" s="86" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="85"/>
+      <c r="B7" s="86" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="85"/>
+      <c r="B8" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="85"/>
+      <c r="B9" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="85"/>
+      <c r="B10" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="85"/>
+      <c r="B11" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="85"/>
+      <c r="B13" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="85"/>
+      <c r="B14" s="86" t="s">
+        <v>602</v>
+      </c>
+      <c r="C14" s="39"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="85"/>
+      <c r="B15" s="87" t="s">
+        <v>605</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="85"/>
+      <c r="B16" s="87" t="s">
+        <v>606</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="85"/>
+      <c r="B17" s="87" t="s">
+        <v>608</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="85"/>
+      <c r="B18" s="87" t="s">
+        <v>607</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="85"/>
+      <c r="B19" s="87" t="s">
+        <v>610</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="85"/>
+      <c r="B20" s="87" t="s">
+        <v>609</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="85"/>
+      <c r="B21" s="87" t="s">
+        <v>612</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="85"/>
+      <c r="B22" s="87" t="s">
+        <v>611</v>
+      </c>
+      <c r="C22" s="39"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="85"/>
+      <c r="B23" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="85"/>
+      <c r="B24" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="85"/>
+      <c r="B25" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="47" t="s">
+        <v>604</v>
+      </c>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="85"/>
+      <c r="B27" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="85"/>
+      <c r="B28" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="85"/>
+      <c r="B29" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="39" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="85"/>
+      <c r="B30" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="85"/>
+      <c r="B31" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="85"/>
+      <c r="B32" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="45"/>
+      <c r="B37" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C37" s="38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
-      <c r="B6" s="38" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="45"/>
+      <c r="B38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C38" s="38" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="45"/>
-      <c r="B7" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
-      <c r="B8" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
-      <c r="B10" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
-      <c r="B12" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
-      <c r="B13" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
-      <c r="B14" s="38" t="s">
-        <v>347</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
-      <c r="B15" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="48"/>
-      <c r="B16" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
-      <c r="B17" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" s="49"/>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="49" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
-      <c r="B19" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
-      <c r="B20" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="C20" s="38"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
-      <c r="B22" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="48"/>
-      <c r="B23" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="48"/>
-      <c r="B24" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="48"/>
-      <c r="B25" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="60" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C27" s="61" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C28" s="61" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C29" s="61" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C30" s="63" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C31" s="63" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C32" s="63" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C33" s="63" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="50"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="50"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="51"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="50"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="53"/>
-      <c r="C37" s="54"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="45"/>
       <c r="B39" s="38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="45"/>
       <c r="B40" s="38" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="45"/>
-      <c r="B41" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>174</v>
-      </c>
+      <c r="A41" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="45"/>
-      <c r="B42" s="38" t="s">
+      <c r="A42" s="46"/>
+      <c r="B42" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="48"/>
+      <c r="B44" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="48"/>
+      <c r="B45" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="48"/>
+      <c r="B46" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="C46" s="38" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="48"/>
+      <c r="B47" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="B43" s="58"/>
-      <c r="C43" s="58"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="46"/>
-      <c r="B44" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="46"/>
-      <c r="B46" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="46"/>
-      <c r="B47" s="38" t="s">
-        <v>14</v>
-      </c>
       <c r="C47" s="38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="46"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="48"/>
       <c r="B48" s="38" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>17</v>
+        <v>542</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="46"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="38" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="46"/>
-      <c r="B50" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="38"/>
+        <v>142</v>
+      </c>
+      <c r="C49" s="49"/>
+    </row>
+    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="48"/>
+      <c r="B50" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="49" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="46"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="57" t="s">
-        <v>147</v>
-      </c>
-      <c r="C51" s="38" t="s">
-        <v>159</v>
+        <v>45</v>
+      </c>
+      <c r="C51" s="49" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="46"/>
-      <c r="B52" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="C52" s="38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="46"/>
+      <c r="A52" s="48"/>
+      <c r="B52" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" s="38"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="48"/>
       <c r="B53" s="57" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C53" s="38" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="46"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="57" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="46"/>
-      <c r="B55" s="57" t="s">
-        <v>151</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="48"/>
+      <c r="B55" s="38" t="s">
+        <v>29</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="46"/>
-      <c r="B56" s="57" t="s">
-        <v>152</v>
+      <c r="A56" s="48"/>
+      <c r="B56" s="38" t="s">
+        <v>30</v>
       </c>
       <c r="C56" s="38" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="46"/>
-      <c r="B57" s="57" t="s">
-        <v>153</v>
+      <c r="A57" s="48"/>
+      <c r="B57" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="C57" s="38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="46"/>
-      <c r="B58" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="C58" s="38" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="46"/>
-      <c r="B59" s="57" t="s">
-        <v>155</v>
-      </c>
-      <c r="C59" s="38" t="s">
-        <v>158</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B58" s="60"/>
+      <c r="C58" s="60"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C59" s="61" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="60" t="s">
-        <v>203</v>
-      </c>
-      <c r="B60" s="60"/>
-      <c r="C60" s="60"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C60" s="61" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
       <c r="B61" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C61" s="63" t="s">
-        <v>207</v>
+      <c r="C61" s="61" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
       <c r="B62" s="8" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C62" s="63" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="50"/>
-      <c r="B63" s="51"/>
-      <c r="C63" s="51"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="50"/>
-      <c r="B64" s="51"/>
-      <c r="C64" s="51"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="50"/>
-      <c r="B65" s="51"/>
-      <c r="C65" s="51"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="9"/>
+      <c r="B63" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" s="63" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="9"/>
+      <c r="B64" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C64" s="63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="9"/>
+      <c r="B65" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" s="63" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="52" t="s">
-        <v>165</v>
-      </c>
-      <c r="B66" s="53"/>
-      <c r="C66" s="54"/>
+      <c r="A66" s="50"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="51"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="44" t="s">
+      <c r="A67" s="50"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="51"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="50"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="53"/>
+      <c r="C69" s="54"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="44"/>
-      <c r="C67" s="44"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="45"/>
-      <c r="B68" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="C68" s="38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="45"/>
-      <c r="B69" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" s="38" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="45"/>
-      <c r="B70" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C70" s="38" t="s">
-        <v>8</v>
-      </c>
+      <c r="B70" s="44"/>
+      <c r="C70" s="44"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="45"/>
       <c r="B71" s="38" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>168</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="45"/>
       <c r="B72" s="38" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="45"/>
       <c r="B73" s="38" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="C73" s="38" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="58" t="s">
+      <c r="A74" s="45"/>
+      <c r="B74" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="B74" s="58"/>
-      <c r="C74" s="58"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="46"/>
-      <c r="B75" s="39" t="s">
+      <c r="B75" s="58"/>
+      <c r="C75" s="58"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="46"/>
+      <c r="B76" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="38" t="s">
+      <c r="C76" s="38" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="47" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="B76" s="47"/>
-      <c r="C76" s="47"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="45"/>
-      <c r="B77" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="C77" s="38" t="s">
+      <c r="B77" s="47"/>
+      <c r="C77" s="47"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="46"/>
+      <c r="B78" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="45"/>
-      <c r="B78" s="38" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="46"/>
+      <c r="B79" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C78" s="38" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="45"/>
-      <c r="B79" s="38" t="s">
-        <v>63</v>
-      </c>
       <c r="C79" s="38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="45"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="46"/>
       <c r="B80" s="38" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C80" s="38" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="45"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="46"/>
       <c r="B81" s="38" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C81" s="38" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="45"/>
-      <c r="B82" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="C82" s="38" t="s">
-        <v>172</v>
-      </c>
+      <c r="A82" s="46"/>
+      <c r="B82" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C82" s="38"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="45"/>
-      <c r="B83" s="38" t="s">
-        <v>67</v>
+      <c r="A83" s="46"/>
+      <c r="B83" s="57" t="s">
+        <v>147</v>
       </c>
       <c r="C83" s="38" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="45"/>
+      <c r="A84" s="46"/>
       <c r="B84" s="57" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C84" s="38" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="45"/>
-      <c r="B85" s="38" t="s">
-        <v>0</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="46"/>
+      <c r="B85" s="57" t="s">
+        <v>149</v>
       </c>
       <c r="C85" s="38" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="60" t="s">
+      <c r="A86" s="46"/>
+      <c r="B86" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C86" s="38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="46"/>
+      <c r="B87" s="57" t="s">
+        <v>151</v>
+      </c>
+      <c r="C87" s="38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="46"/>
+      <c r="B88" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C88" s="38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="46"/>
+      <c r="B89" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="C89" s="38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="46"/>
+      <c r="B90" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="C90" s="38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A91" s="46"/>
+      <c r="B91" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="C91" s="38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="60" t="s">
         <v>203</v>
       </c>
-      <c r="B86" s="60"/>
-      <c r="C86" s="60"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9" t="s">
+      <c r="B92" s="60"/>
+      <c r="C92" s="60"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="9"/>
+      <c r="B93" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C87" s="61" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="55"/>
-      <c r="B88" s="56"/>
-      <c r="C88" s="56"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="52" t="s">
-        <v>559</v>
-      </c>
-      <c r="B91" s="53"/>
-      <c r="C91" s="59"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="44" t="s">
+      <c r="C93" s="63" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A94" s="9"/>
+      <c r="B94" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C94" s="63" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="50"/>
+      <c r="B95" s="51"/>
+      <c r="C95" s="51"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="50"/>
+      <c r="B96" s="51"/>
+      <c r="C96" s="51"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="50"/>
+      <c r="B97" s="51"/>
+      <c r="C97" s="51"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="B98" s="53"/>
+      <c r="C98" s="54"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B92" s="44"/>
-      <c r="C92" s="44"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="45"/>
-      <c r="B93" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="C93" s="38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="45"/>
-      <c r="B94" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C94" s="38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="45"/>
-      <c r="B95" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C95" s="38" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="45"/>
-      <c r="B96" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C96" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="B97" s="58"/>
-      <c r="C97" s="58"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="46"/>
-      <c r="B98" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C98" s="38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B99" s="47"/>
-      <c r="C99" s="47"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="44"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="45"/>
       <c r="B100" s="38" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C100" s="38" t="s">
         <v>15</v>
@@ -6694,711 +6878,963 @@
         <v>14</v>
       </c>
       <c r="C101" s="38" t="s">
-        <v>16</v>
+        <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="46"/>
+      <c r="A102" s="45"/>
       <c r="B102" s="38" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C102" s="38" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="46"/>
+      <c r="A103" s="45"/>
       <c r="B103" s="38" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C103" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A104" s="46"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="45"/>
       <c r="B104" s="38" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C104" s="38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="46"/>
-      <c r="B105" s="57" t="s">
-        <v>179</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A105" s="45"/>
+      <c r="B105" s="38" t="s">
+        <v>67</v>
       </c>
       <c r="C105" s="38" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="46"/>
-      <c r="B106" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="C106" s="38" t="s">
-        <v>199</v>
-      </c>
+      <c r="A106" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B106" s="58"/>
+      <c r="C106" s="58"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="46"/>
-      <c r="B107" s="57" t="s">
-        <v>183</v>
+      <c r="B107" s="39" t="s">
+        <v>7</v>
       </c>
       <c r="C107" s="38" t="s">
-        <v>192</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="46"/>
-      <c r="B108" s="57" t="s">
-        <v>184</v>
-      </c>
-      <c r="C108" s="38" t="s">
-        <v>193</v>
-      </c>
+      <c r="A108" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B108" s="47"/>
+      <c r="C108" s="47"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="46"/>
-      <c r="B109" s="57" t="s">
-        <v>181</v>
+      <c r="A109" s="45"/>
+      <c r="B109" s="38" t="s">
+        <v>166</v>
       </c>
       <c r="C109" s="38" t="s">
-        <v>194</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="46"/>
-      <c r="B110" s="57" t="s">
-        <v>182</v>
+      <c r="A110" s="45"/>
+      <c r="B110" s="38" t="s">
+        <v>14</v>
       </c>
       <c r="C110" s="38" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="46"/>
-      <c r="B111" s="57" t="s">
-        <v>185</v>
+      <c r="A111" s="45"/>
+      <c r="B111" s="38" t="s">
+        <v>63</v>
       </c>
       <c r="C111" s="38" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="46"/>
-      <c r="B112" s="57" t="s">
-        <v>186</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="45"/>
+      <c r="B112" s="38" t="s">
+        <v>10</v>
       </c>
       <c r="C112" s="38" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="46"/>
-      <c r="B113" s="57" t="s">
-        <v>187</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="45"/>
+      <c r="B113" s="38" t="s">
+        <v>66</v>
       </c>
       <c r="C113" s="38" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="46"/>
+      <c r="A114" s="45"/>
       <c r="B114" s="57" t="s">
-        <v>188</v>
+        <v>65</v>
       </c>
       <c r="C114" s="38" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="46"/>
-      <c r="B115" s="57" t="s">
-        <v>189</v>
+      <c r="A115" s="45"/>
+      <c r="B115" s="38" t="s">
+        <v>67</v>
       </c>
       <c r="C115" s="38" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="46"/>
+      <c r="A116" s="45"/>
       <c r="B116" s="57" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="C116" s="38" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="60" t="s">
+      <c r="A117" s="45"/>
+      <c r="B117" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="60" t="s">
         <v>203</v>
       </c>
-      <c r="B117" s="60"/>
-      <c r="C117" s="60"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="9"/>
-      <c r="B118" s="9" t="s">
+      <c r="B118" s="60"/>
+      <c r="C118" s="60"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="9"/>
+      <c r="B119" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C118" s="61" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="50"/>
-      <c r="B119" s="51"/>
-      <c r="C119" s="51"/>
+      <c r="C119" s="61" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="50"/>
-      <c r="B120" s="51"/>
-      <c r="C120" s="51"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="50"/>
-      <c r="B121" s="51"/>
-      <c r="C121" s="51"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="B122" s="53"/>
-      <c r="C122" s="54"/>
+      <c r="A120" s="55"/>
+      <c r="B120" s="56"/>
+      <c r="C120" s="56"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="44" t="s">
+      <c r="A123" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="B123" s="53"/>
+      <c r="C123" s="59"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B123" s="44"/>
-      <c r="C123" s="44"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="45"/>
-      <c r="B124" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="C124" s="38" t="s">
-        <v>22</v>
-      </c>
+      <c r="B124" s="44"/>
+      <c r="C124" s="44"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="45"/>
       <c r="B125" s="38" t="s">
-        <v>20</v>
+        <v>177</v>
       </c>
       <c r="C125" s="38" t="s">
-        <v>227</v>
+        <v>15</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="45"/>
       <c r="B126" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C126" s="38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="45"/>
+      <c r="B127" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C127" s="38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="45"/>
+      <c r="B128" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C126" s="38" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="58" t="s">
+      <c r="C128" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="B127" s="58"/>
-      <c r="C127" s="58"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="46"/>
-      <c r="B128" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C128" s="38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B129" s="47"/>
-      <c r="C129" s="47"/>
+      <c r="B129" s="58"/>
+      <c r="C129" s="58"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="46"/>
-      <c r="B130" s="38" t="s">
+      <c r="B130" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" s="38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B131" s="47"/>
+      <c r="C131" s="47"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="45"/>
+      <c r="B132" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="C130" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="46"/>
-      <c r="B131" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C131" s="38"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="46"/>
-      <c r="B132" s="57" t="s">
-        <v>228</v>
-      </c>
       <c r="C132" s="38" t="s">
-        <v>363</v>
+        <v>15</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="46"/>
-      <c r="B133" s="57" t="s">
-        <v>229</v>
+      <c r="A133" s="45"/>
+      <c r="B133" s="38" t="s">
+        <v>14</v>
       </c>
       <c r="C133" s="38" t="s">
-        <v>364</v>
+        <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="46"/>
-      <c r="B134" s="57" t="s">
-        <v>230</v>
+      <c r="B134" s="38" t="s">
+        <v>71</v>
       </c>
       <c r="C134" s="38" t="s">
-        <v>368</v>
+        <v>18</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="46"/>
-      <c r="B135" s="57" t="s">
-        <v>236</v>
+      <c r="B135" s="38" t="s">
+        <v>0</v>
       </c>
       <c r="C135" s="38" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="46"/>
-      <c r="B136" s="57" t="s">
-        <v>148</v>
+      <c r="B136" s="38" t="s">
+        <v>1</v>
       </c>
       <c r="C136" s="38" t="s">
-        <v>365</v>
+        <v>19</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="46"/>
       <c r="B137" s="57" t="s">
-        <v>231</v>
+        <v>179</v>
       </c>
       <c r="C137" s="38" t="s">
-        <v>370</v>
+        <v>191</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="46"/>
       <c r="B138" s="57" t="s">
-        <v>232</v>
+        <v>180</v>
       </c>
       <c r="C138" s="38" t="s">
-        <v>366</v>
+        <v>199</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="46"/>
       <c r="B139" s="57" t="s">
-        <v>233</v>
+        <v>183</v>
       </c>
       <c r="C139" s="38" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="46"/>
       <c r="B140" s="57" t="s">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="C140" s="38" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="46"/>
       <c r="B141" s="57" t="s">
-        <v>235</v>
+        <v>181</v>
       </c>
       <c r="C141" s="38" t="s">
-        <v>372</v>
+        <v>194</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="46"/>
-      <c r="B142" s="38" t="s">
-        <v>20</v>
+      <c r="B142" s="57" t="s">
+        <v>182</v>
       </c>
       <c r="C142" s="38" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="46"/>
-      <c r="B143" s="38" t="s">
-        <v>0</v>
+      <c r="B143" s="57" t="s">
+        <v>185</v>
       </c>
       <c r="C143" s="38" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="46"/>
-      <c r="B144" s="38" t="s">
-        <v>224</v>
+      <c r="B144" s="57" t="s">
+        <v>186</v>
       </c>
       <c r="C144" s="38" t="s">
-        <v>373</v>
+        <v>197</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="46"/>
       <c r="B145" s="57" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
       <c r="C145" s="38" t="s">
-        <v>374</v>
+        <v>198</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="46"/>
       <c r="B146" s="57" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="C146" s="38" t="s">
-        <v>375</v>
+        <v>200</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="46"/>
-      <c r="B147" s="38" t="s">
-        <v>378</v>
+      <c r="B147" s="57" t="s">
+        <v>189</v>
       </c>
       <c r="C147" s="38" t="s">
-        <v>379</v>
+        <v>201</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="46"/>
       <c r="B148" s="57" t="s">
-        <v>377</v>
+        <v>190</v>
       </c>
       <c r="C148" s="38" t="s">
-        <v>380</v>
+        <v>202</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="46"/>
-      <c r="B149" s="57" t="s">
-        <v>376</v>
-      </c>
-      <c r="C149" s="38" t="s">
-        <v>381</v>
-      </c>
+      <c r="A149" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B149" s="60"/>
+      <c r="C149" s="60"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="46"/>
-      <c r="B150" s="38" t="s">
-        <v>349</v>
-      </c>
-      <c r="C150" s="38" t="s">
-        <v>382</v>
+      <c r="A150" s="9"/>
+      <c r="B150" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C150" s="61" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="46"/>
-      <c r="B151" s="38" t="s">
-        <v>350</v>
-      </c>
-      <c r="C151" s="38" t="s">
-        <v>383</v>
-      </c>
+      <c r="A151" s="50"/>
+      <c r="B151" s="51"/>
+      <c r="C151" s="51"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="46"/>
-      <c r="B152" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="C152" s="38" t="s">
-        <v>21</v>
-      </c>
+      <c r="A152" s="50"/>
+      <c r="B152" s="51"/>
+      <c r="C152" s="51"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="60" t="s">
-        <v>203</v>
-      </c>
-      <c r="B153" s="60"/>
-      <c r="C153" s="60"/>
+      <c r="A153" s="50"/>
+      <c r="B153" s="51"/>
+      <c r="C153" s="51"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="9"/>
-      <c r="B154" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="C154" s="62" t="s">
-        <v>221</v>
+      <c r="A154" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" s="53"/>
+      <c r="C154" s="54"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B155" s="44"/>
+      <c r="C155" s="44"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="45"/>
+      <c r="B156" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C156" s="38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="45"/>
+      <c r="B157" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C157" s="38" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" s="52" t="s">
-        <v>250</v>
-      </c>
-      <c r="B158" s="53"/>
-      <c r="C158" s="54"/>
+      <c r="A158" s="45"/>
+      <c r="B158" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="38" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B159" s="44"/>
-      <c r="C159" s="44"/>
+      <c r="A159" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B159" s="58"/>
+      <c r="C159" s="58"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="45"/>
-      <c r="B160" s="38" t="s">
-        <v>251</v>
+      <c r="A160" s="46"/>
+      <c r="B160" s="39" t="s">
+        <v>7</v>
       </c>
       <c r="C160" s="38" t="s">
-        <v>252</v>
+        <v>137</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="45"/>
-      <c r="B161" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="C161" s="38" t="s">
-        <v>253</v>
-      </c>
+      <c r="A161" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B161" s="47"/>
+      <c r="C161" s="47"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="45"/>
+      <c r="A162" s="46"/>
       <c r="B162" s="38" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="C162" s="38" t="s">
-        <v>254</v>
+        <v>22</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="B163" s="58"/>
-      <c r="C163" s="58"/>
+      <c r="A163" s="46"/>
+      <c r="B163" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C163" s="38"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="46"/>
-      <c r="B164" s="39" t="s">
-        <v>7</v>
+      <c r="B164" s="57" t="s">
+        <v>228</v>
       </c>
       <c r="C164" s="38" t="s">
-        <v>137</v>
+        <v>363</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B165" s="47"/>
-      <c r="C165" s="47"/>
+      <c r="A165" s="46"/>
+      <c r="B165" s="57" t="s">
+        <v>229</v>
+      </c>
+      <c r="C165" s="38" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="46"/>
-      <c r="B166" s="38" t="s">
-        <v>251</v>
+      <c r="B166" s="57" t="s">
+        <v>230</v>
       </c>
       <c r="C166" s="38" t="s">
-        <v>252</v>
+        <v>368</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="46"/>
-      <c r="B167" s="38" t="s">
-        <v>248</v>
+      <c r="B167" s="57" t="s">
+        <v>236</v>
       </c>
       <c r="C167" s="38" t="s">
-        <v>255</v>
+        <v>369</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="46"/>
-      <c r="B168" s="38" t="s">
+      <c r="B168" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="C168" s="38" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="46"/>
+      <c r="B169" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="C169" s="38" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="46"/>
+      <c r="B170" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="C170" s="38" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="46"/>
+      <c r="B171" s="57" t="s">
+        <v>233</v>
+      </c>
+      <c r="C171" s="38" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A172" s="46"/>
+      <c r="B172" s="57" t="s">
+        <v>234</v>
+      </c>
+      <c r="C172" s="38" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A173" s="46"/>
+      <c r="B173" s="57" t="s">
+        <v>235</v>
+      </c>
+      <c r="C173" s="38" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="46"/>
+      <c r="B174" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C174" s="38" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="46"/>
+      <c r="B175" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C168" s="38" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" s="60" t="s">
-        <v>203</v>
-      </c>
-      <c r="B169" s="60"/>
-      <c r="C169" s="60"/>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" s="9"/>
-      <c r="B170" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="C170" s="62" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" s="52" t="s">
-        <v>249</v>
-      </c>
-      <c r="B174" s="53"/>
-      <c r="C174" s="54"/>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B175" s="44"/>
-      <c r="C175" s="44"/>
+      <c r="C175" s="38" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" s="45"/>
+      <c r="A176" s="46"/>
       <c r="B176" s="38" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="C176" s="38" t="s">
-        <v>260</v>
+        <v>373</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" s="45"/>
-      <c r="B177" s="38" t="s">
-        <v>243</v>
+      <c r="A177" s="46"/>
+      <c r="B177" s="57" t="s">
+        <v>237</v>
       </c>
       <c r="C177" s="38" t="s">
-        <v>261</v>
+        <v>374</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A178" s="45"/>
-      <c r="B178" s="38" t="s">
-        <v>244</v>
+      <c r="A178" s="46"/>
+      <c r="B178" s="57" t="s">
+        <v>238</v>
       </c>
       <c r="C178" s="38" t="s">
-        <v>262</v>
+        <v>375</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="45"/>
+      <c r="A179" s="46"/>
       <c r="B179" s="38" t="s">
-        <v>246</v>
+        <v>378</v>
       </c>
       <c r="C179" s="38" t="s">
-        <v>263</v>
+        <v>379</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="B180" s="58"/>
-      <c r="C180" s="58"/>
+      <c r="A180" s="46"/>
+      <c r="B180" s="57" t="s">
+        <v>377</v>
+      </c>
+      <c r="C180" s="38" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="46"/>
-      <c r="B181" s="39" t="s">
-        <v>7</v>
+      <c r="B181" s="57" t="s">
+        <v>376</v>
       </c>
       <c r="C181" s="38" t="s">
-        <v>137</v>
+        <v>381</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B182" s="47"/>
-      <c r="C182" s="47"/>
+      <c r="A182" s="46"/>
+      <c r="B182" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="C182" s="38" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="46"/>
       <c r="B183" s="38" t="s">
-        <v>259</v>
+        <v>350</v>
       </c>
       <c r="C183" s="38" t="s">
-        <v>260</v>
+        <v>383</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="46"/>
       <c r="B184" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="C184" s="38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B185" s="60"/>
+      <c r="C185" s="60"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="9"/>
+      <c r="B186" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C186" s="62" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="52" t="s">
+        <v>250</v>
+      </c>
+      <c r="B190" s="53"/>
+      <c r="C190" s="54"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B191" s="44"/>
+      <c r="C191" s="44"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="45"/>
+      <c r="B192" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="C192" s="38" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="45"/>
+      <c r="B193" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="C193" s="38" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="45"/>
+      <c r="B194" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C194" s="38" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B195" s="58"/>
+      <c r="C195" s="58"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="46"/>
+      <c r="B196" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C196" s="38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B197" s="47"/>
+      <c r="C197" s="47"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="46"/>
+      <c r="B198" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="C198" s="38" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="46"/>
+      <c r="B199" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="C199" s="38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="46"/>
+      <c r="B200" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C200" s="38" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B201" s="60"/>
+      <c r="C201" s="60"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="9"/>
+      <c r="B202" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C202" s="62" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" s="52" t="s">
+        <v>249</v>
+      </c>
+      <c r="B206" s="53"/>
+      <c r="C206" s="54"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B207" s="44"/>
+      <c r="C207" s="44"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" s="45"/>
+      <c r="B208" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="C208" s="38" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" s="45"/>
+      <c r="B209" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="C184" s="38" t="s">
+      <c r="C209" s="38" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" s="46"/>
-      <c r="B185" s="38" t="s">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" s="45"/>
+      <c r="B210" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="C185" s="38" t="s">
+      <c r="C210" s="38" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" s="46"/>
-      <c r="B186" s="38" t="s">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" s="45"/>
+      <c r="B211" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="C186" s="38" t="s">
+      <c r="C211" s="38" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" s="60" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B212" s="58"/>
+      <c r="C212" s="58"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" s="46"/>
+      <c r="B213" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C213" s="38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B214" s="47"/>
+      <c r="C214" s="47"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A215" s="46"/>
+      <c r="B215" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="C215" s="38" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A216" s="46"/>
+      <c r="B216" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="C216" s="38" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" s="46"/>
+      <c r="B217" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C217" s="38" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" s="46"/>
+      <c r="B218" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="C218" s="38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" s="60" t="s">
         <v>203</v>
       </c>
-      <c r="B187" s="60"/>
-      <c r="C187" s="60"/>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188" s="9"/>
-      <c r="B188" s="9" t="s">
+      <c r="B219" s="60"/>
+      <c r="C219" s="60"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" s="9"/>
+      <c r="B220" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C188" s="62" t="s">
+      <c r="C220" s="62" t="s">
         <v>258</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C118" r:id="rId1"/>
-    <hyperlink ref="C87" r:id="rId2"/>
-    <hyperlink ref="C61" r:id="rId3"/>
-    <hyperlink ref="C62" r:id="rId4" location="section_11.1" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - section_11.1"/>
-    <hyperlink ref="C27" r:id="rId5"/>
-    <hyperlink ref="C28" r:id="rId6"/>
-    <hyperlink ref="C29" r:id="rId7"/>
-    <hyperlink ref="C30" r:id="rId8" location="section_9.2" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - section_9.2"/>
-    <hyperlink ref="C32" r:id="rId9" location="section_11.2" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - section_11.2"/>
-    <hyperlink ref="C33" r:id="rId10" location="section_11.2" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - section_11.2"/>
-    <hyperlink ref="C31" r:id="rId11" location="table_10-2" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - table_10-2"/>
-    <hyperlink ref="C154" r:id="rId12"/>
-    <hyperlink ref="C170" r:id="rId13"/>
-    <hyperlink ref="C188" r:id="rId14"/>
+    <hyperlink ref="C150" r:id="rId1"/>
+    <hyperlink ref="C119" r:id="rId2"/>
+    <hyperlink ref="C93" r:id="rId3"/>
+    <hyperlink ref="C94" r:id="rId4" location="section_11.1" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - section_11.1"/>
+    <hyperlink ref="C59" r:id="rId5"/>
+    <hyperlink ref="C60" r:id="rId6"/>
+    <hyperlink ref="C61" r:id="rId7"/>
+    <hyperlink ref="C62" r:id="rId8" location="section_9.2" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - section_9.2"/>
+    <hyperlink ref="C64" r:id="rId9" location="section_11.2" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - section_11.2"/>
+    <hyperlink ref="C65" r:id="rId10" location="section_11.2" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - section_11.2"/>
+    <hyperlink ref="C63" r:id="rId11" location="table_10-2" display="https://reference.niem.gov/niem/specification/naming-and-design-rules/4.0/niem-ndr-4.0.html - table_10-2"/>
+    <hyperlink ref="C186" r:id="rId12"/>
+    <hyperlink ref="C202" r:id="rId13"/>
+    <hyperlink ref="C220" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId15"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7409,11 +7845,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7498,26 +7932,28 @@
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="83" t="s">
+        <v>602</v>
+      </c>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
       <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -7525,51 +7961,51 @@
       <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="22"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B20" s="27" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
-        <v>96</v>
       </c>
       <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
       <c r="B26" s="6"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -7577,12 +8013,21 @@
       <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="22"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B29" s="6"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
+      <formula1>MAPPING_ARTIFACTS</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="3">
@@ -7606,7 +8051,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7632,13 +8077,13 @@
         <v>47</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>49</v>
@@ -7653,19 +8098,19 @@
         <v>48</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>347</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>569</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>346</v>
@@ -7847,7 +8292,7 @@
         <v>392</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>436</v>
@@ -8303,7 +8748,7 @@
         <v>450</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>451</v>
@@ -8624,7 +9069,7 @@
         <v>501</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>505</v>
@@ -8719,7 +9164,7 @@
         <v>520</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>522</v>
@@ -8760,7 +9205,7 @@
         <v>523</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -8890,7 +9335,7 @@
         <v>450</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>451</v>
@@ -9111,9 +9556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9136,13 +9581,13 @@
         <v>47</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>553</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>554</v>
       </c>
       <c r="E1" s="30" t="s">
         <v>69</v>
@@ -9157,16 +9602,16 @@
         <v>48</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -9233,7 +9678,7 @@
         <v>301</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>533</v>
+        <v>640</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -9510,9 +9955,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9540,19 +9985,19 @@
         <v>62</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>570</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>571</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>572</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>49</v>
@@ -9567,19 +10012,19 @@
         <v>64</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="N1" s="19" t="s">
         <v>345</v>
       </c>
       <c r="O1" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>344</v>
@@ -9989,7 +10434,7 @@
         <v>339</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>339</v>
@@ -10013,7 +10458,7 @@
         <v>339</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>339</v>
@@ -10105,7 +10550,7 @@
         <v>339</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>339</v>
@@ -10153,7 +10598,7 @@
         <v>339</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>339</v>
@@ -10177,7 +10622,7 @@
         <v>339</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>339</v>
@@ -10226,7 +10671,7 @@
         <v>339</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>339</v>
@@ -10250,7 +10695,7 @@
         <v>339</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>339</v>
@@ -10319,7 +10764,7 @@
         <v>339</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>339</v>
@@ -10370,7 +10815,7 @@
         <v>339</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -10393,7 +10838,7 @@
         <v>339</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -10434,7 +10879,7 @@
         <v>339</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>339</v>
@@ -10458,7 +10903,7 @@
         <v>339</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>339</v>
@@ -10578,7 +11023,7 @@
         <v>339</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -10601,7 +11046,7 @@
         <v>339</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -10676,7 +11121,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10702,19 +11147,19 @@
         <v>68</v>
       </c>
       <c r="B1" s="77" t="s">
+        <v>559</v>
+      </c>
+      <c r="C1" s="78" t="s">
         <v>560</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="D1" s="78" t="s">
+        <v>553</v>
+      </c>
+      <c r="E1" s="78" t="s">
         <v>561</v>
       </c>
-      <c r="D1" s="78" t="s">
-        <v>554</v>
-      </c>
-      <c r="E1" s="78" t="s">
-        <v>562</v>
-      </c>
       <c r="F1" s="79" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G1" s="79" t="s">
         <v>50</v>
@@ -10726,16 +11171,16 @@
         <v>70</v>
       </c>
       <c r="J1" s="81" t="s">
+        <v>562</v>
+      </c>
+      <c r="K1" s="82" t="s">
         <v>563</v>
       </c>
-      <c r="K1" s="82" t="s">
+      <c r="L1" s="82" t="s">
+        <v>556</v>
+      </c>
+      <c r="M1" s="82" t="s">
         <v>564</v>
-      </c>
-      <c r="L1" s="82" t="s">
-        <v>557</v>
-      </c>
-      <c r="M1" s="82" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -10792,7 +11237,7 @@
         <v>338</v>
       </c>
       <c r="L3" s="75" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="M3" s="75"/>
     </row>
@@ -10882,10 +11327,10 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10913,10 +11358,10 @@
         <v>222</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>69</v>
@@ -10931,28 +11376,28 @@
         <v>223</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>575</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>576</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>577</v>
-      </c>
       <c r="J1" s="13" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>348</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="66" t="s">
         <v>580</v>
-      </c>
-      <c r="O1" s="66" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -11038,16 +11483,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>49</v>
@@ -11062,13 +11507,13 @@
         <v>48</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="J1" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>596</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated template and valid example spreadsheets
</commit_message>
<xml_diff>
--- a/public/examples/iepd-requirements-example.xlsx
+++ b/public/examples/iepd-requirements-example.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="647">
   <si>
     <t>Definition</t>
   </si>
@@ -3390,6 +3390,24 @@
   </si>
   <si>
     <t>no match</t>
+  </si>
+  <si>
+    <t>Movie Info exchange</t>
+  </si>
+  <si>
+    <t>Movie Info IEPD</t>
+  </si>
+  <si>
+    <t>NIEM 4.1</t>
+  </si>
+  <si>
+    <t>Uses movie-related components from schema.org as source requirements for a movie info NIEM IEPD.</t>
+  </si>
+  <si>
+    <t>https://schema.org/Movie</t>
+  </si>
+  <si>
+    <t>https://schema.org</t>
   </si>
 </sst>
 </file>
@@ -3571,6 +3589,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3755,7 +3774,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3768,9 +3787,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3820,23 +3836,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3992,6 +3999,15 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -4774,6 +4790,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4795,6 +4812,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4816,6 +4834,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5502,48 +5521,48 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" style="21" customWidth="1"/>
-    <col min="3" max="4" width="35" style="15" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="15"/>
+    <col min="1" max="1" width="28.6640625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" style="20" customWidth="1"/>
+    <col min="3" max="4" width="35" style="14" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="37" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="28" t="s">
         <v>108</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -5551,13 +5570,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="28" t="s">
         <v>120</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -5565,13 +5584,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="28" t="s">
         <v>115</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -5579,13 +5598,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="28" t="s">
         <v>116</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -5593,13 +5612,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="28" t="s">
         <v>117</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -5607,13 +5626,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="28" t="s">
         <v>96</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -5621,13 +5640,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="28" t="s">
         <v>104</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -5635,13 +5654,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="28" t="s">
         <v>123</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -5649,253 +5668,253 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="42" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="38" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="27" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="27" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="27" t="s">
         <v>534</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="27" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="33" t="s">
         <v>640</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="35" t="s">
         <v>533</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="27" t="s">
         <v>534</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="27" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="27" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="33" t="s">
         <v>609</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="35" t="s">
         <v>613</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="27" t="s">
         <v>615</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="27" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="27" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="31" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="47" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="47" t="s">
         <v>546</v>
       </c>
-      <c r="B39" s="51" t="s">
+      <c r="B39" s="47" t="s">
         <v>547</v>
       </c>
     </row>
@@ -5934,37 +5953,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>600</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>589</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>591</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>592</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>593</v>
       </c>
     </row>
@@ -6007,37 +6026,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>581</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>586</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>587</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>582</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>583</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>584</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>585</v>
       </c>
     </row>
@@ -6063,1756 +6082,1756 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="76" style="21" customWidth="1"/>
-    <col min="4" max="5" width="29.21875" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="20"/>
+    <col min="1" max="1" width="3.6640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="76" style="20" customWidth="1"/>
+    <col min="4" max="5" width="29.21875" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="80" t="s">
         <v>601</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="40" t="s">
         <v>603</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="85"/>
-      <c r="B5" s="86" t="s">
+      <c r="A5" s="81"/>
+      <c r="B5" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="35" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="85"/>
-      <c r="B6" s="86" t="s">
+      <c r="A6" s="81"/>
+      <c r="B6" s="82" t="s">
         <v>264</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="35" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="85"/>
-      <c r="B7" s="86" t="s">
+      <c r="A7" s="81"/>
+      <c r="B7" s="82" t="s">
         <v>265</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="35" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="85"/>
-      <c r="B8" s="86" t="s">
+      <c r="A8" s="81"/>
+      <c r="B8" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="35" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86" t="s">
+      <c r="A9" s="81"/>
+      <c r="B9" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="35" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="85"/>
-      <c r="B10" s="86" t="s">
+      <c r="A10" s="81"/>
+      <c r="B10" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="35" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="85"/>
-      <c r="B11" s="86" t="s">
+      <c r="A11" s="81"/>
+      <c r="B11" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="35" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="85"/>
-      <c r="B13" s="86" t="s">
+      <c r="A13" s="81"/>
+      <c r="B13" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="35" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="85"/>
-      <c r="B14" s="86" t="s">
+      <c r="A14" s="81"/>
+      <c r="B14" s="82" t="s">
         <v>602</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="35"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="85"/>
-      <c r="B15" s="87" t="s">
+      <c r="A15" s="81"/>
+      <c r="B15" s="83" t="s">
         <v>605</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="35" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="85"/>
-      <c r="B16" s="87" t="s">
+      <c r="A16" s="81"/>
+      <c r="B16" s="83" t="s">
         <v>606</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="35" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="85"/>
-      <c r="B17" s="87" t="s">
+      <c r="A17" s="81"/>
+      <c r="B17" s="83" t="s">
         <v>608</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="35" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="85"/>
-      <c r="B18" s="87" t="s">
+      <c r="A18" s="81"/>
+      <c r="B18" s="83" t="s">
         <v>607</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="35" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="85"/>
-      <c r="B19" s="87" t="s">
+      <c r="A19" s="81"/>
+      <c r="B19" s="83" t="s">
         <v>610</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="35" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="85"/>
-      <c r="B20" s="87" t="s">
+      <c r="A20" s="81"/>
+      <c r="B20" s="83" t="s">
         <v>609</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="35" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="85"/>
-      <c r="B21" s="87" t="s">
+      <c r="A21" s="81"/>
+      <c r="B21" s="83" t="s">
         <v>612</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="35" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="85"/>
-      <c r="B22" s="87" t="s">
+      <c r="A22" s="81"/>
+      <c r="B22" s="83" t="s">
         <v>611</v>
       </c>
-      <c r="C22" s="39"/>
+      <c r="C22" s="35"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="85"/>
-      <c r="B23" s="86" t="s">
+      <c r="A23" s="81"/>
+      <c r="B23" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="35" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="85"/>
-      <c r="B24" s="86" t="s">
+      <c r="A24" s="81"/>
+      <c r="B24" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="35" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="85"/>
-      <c r="B25" s="86" t="s">
+      <c r="A25" s="81"/>
+      <c r="B25" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="35" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="43" t="s">
         <v>604</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="85"/>
-      <c r="B27" s="86" t="s">
+      <c r="A27" s="81"/>
+      <c r="B27" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="35" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="85"/>
-      <c r="B28" s="86" t="s">
+      <c r="A28" s="81"/>
+      <c r="B28" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="35" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="85"/>
-      <c r="B29" s="86" t="s">
+      <c r="A29" s="81"/>
+      <c r="B29" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="35" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="85"/>
-      <c r="B30" s="86" t="s">
+      <c r="A30" s="81"/>
+      <c r="B30" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="35" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="85"/>
-      <c r="B31" s="86" t="s">
+      <c r="A31" s="81"/>
+      <c r="B31" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="35" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="85"/>
-      <c r="B32" s="86" t="s">
+      <c r="A32" s="81"/>
+      <c r="B32" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="35" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="45"/>
-      <c r="B37" s="38" t="s">
+      <c r="A37" s="41"/>
+      <c r="B37" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="45"/>
-      <c r="B38" s="38" t="s">
+      <c r="A38" s="41"/>
+      <c r="B38" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="34" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
-      <c r="B39" s="38" t="s">
+      <c r="A39" s="41"/>
+      <c r="B39" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="38" t="s">
+      <c r="C39" s="34" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
-      <c r="B40" s="38" t="s">
+      <c r="A40" s="41"/>
+      <c r="B40" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="34" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="58" t="s">
+      <c r="A41" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="46"/>
-      <c r="B42" s="39" t="s">
+      <c r="A42" s="42"/>
+      <c r="B42" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="38" t="s">
+      <c r="C42" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="48"/>
-      <c r="B44" s="38" t="s">
+      <c r="A44" s="44"/>
+      <c r="B44" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="C44" s="38" t="s">
+      <c r="C44" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="48"/>
-      <c r="B45" s="38" t="s">
+      <c r="A45" s="44"/>
+      <c r="B45" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="38" t="s">
+      <c r="C45" s="34" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="48"/>
-      <c r="B46" s="38" t="s">
+      <c r="A46" s="44"/>
+      <c r="B46" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C46" s="34" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="48"/>
-      <c r="B47" s="38" t="s">
+      <c r="A47" s="44"/>
+      <c r="B47" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="34" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="48"/>
-      <c r="B48" s="38" t="s">
+      <c r="A48" s="44"/>
+      <c r="B48" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="38" t="s">
+      <c r="C48" s="34" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="48"/>
-      <c r="B49" s="38" t="s">
+      <c r="A49" s="44"/>
+      <c r="B49" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C49" s="49"/>
+      <c r="C49" s="45"/>
     </row>
     <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="48"/>
-      <c r="B50" s="57" t="s">
+      <c r="A50" s="44"/>
+      <c r="B50" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="49" t="s">
+      <c r="C50" s="45" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="48"/>
-      <c r="B51" s="57" t="s">
+      <c r="A51" s="44"/>
+      <c r="B51" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="49" t="s">
+      <c r="C51" s="45" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="48"/>
-      <c r="B52" s="38" t="s">
+      <c r="A52" s="44"/>
+      <c r="B52" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C52" s="38"/>
+      <c r="C52" s="34"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="48"/>
-      <c r="B53" s="57" t="s">
+      <c r="A53" s="44"/>
+      <c r="B53" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="C53" s="38" t="s">
+      <c r="C53" s="34" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="48"/>
-      <c r="B54" s="57" t="s">
+      <c r="A54" s="44"/>
+      <c r="B54" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="38" t="s">
+      <c r="C54" s="34" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="48"/>
-      <c r="B55" s="38" t="s">
+      <c r="A55" s="44"/>
+      <c r="B55" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="38" t="s">
+      <c r="C55" s="34" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="48"/>
-      <c r="B56" s="38" t="s">
+      <c r="A56" s="44"/>
+      <c r="B56" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C56" s="38" t="s">
+      <c r="C56" s="34" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="48"/>
-      <c r="B57" s="38" t="s">
+      <c r="A57" s="44"/>
+      <c r="B57" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="38" t="s">
+      <c r="C57" s="34" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="60" t="s">
+      <c r="A58" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="B58" s="60"/>
-      <c r="C58" s="60"/>
+      <c r="B58" s="56"/>
+      <c r="C58" s="56"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
-      <c r="B59" s="8" t="s">
+      <c r="A59" s="8"/>
+      <c r="B59" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C59" s="61" t="s">
+      <c r="C59" s="57" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
-      <c r="B60" s="8" t="s">
+      <c r="A60" s="8"/>
+      <c r="B60" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="61" t="s">
+      <c r="C60" s="57" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="9"/>
-      <c r="B61" s="8" t="s">
+      <c r="A61" s="8"/>
+      <c r="B61" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C61" s="61" t="s">
+      <c r="C61" s="57" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
-      <c r="B62" s="8" t="s">
+      <c r="A62" s="8"/>
+      <c r="B62" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C62" s="63" t="s">
+      <c r="C62" s="59" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
-      <c r="B63" s="8" t="s">
+      <c r="A63" s="8"/>
+      <c r="B63" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="C63" s="63" t="s">
+      <c r="C63" s="59" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="9"/>
-      <c r="B64" s="8" t="s">
+      <c r="A64" s="8"/>
+      <c r="B64" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C64" s="63" t="s">
+      <c r="C64" s="59" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="9"/>
-      <c r="B65" s="8" t="s">
+      <c r="A65" s="8"/>
+      <c r="B65" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C65" s="63" t="s">
+      <c r="C65" s="59" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="50"/>
-      <c r="B66" s="51"/>
-      <c r="C66" s="51"/>
+      <c r="A66" s="46"/>
+      <c r="B66" s="47"/>
+      <c r="C66" s="47"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="50"/>
-      <c r="B67" s="51"/>
-      <c r="C67" s="51"/>
+      <c r="A67" s="46"/>
+      <c r="B67" s="47"/>
+      <c r="C67" s="47"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="50"/>
-      <c r="B68" s="51"/>
-      <c r="C68" s="51"/>
+      <c r="A68" s="46"/>
+      <c r="B68" s="47"/>
+      <c r="C68" s="47"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="52" t="s">
+      <c r="A69" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="53"/>
-      <c r="C69" s="54"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="50"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="44" t="s">
+      <c r="A70" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B70" s="44"/>
-      <c r="C70" s="44"/>
+      <c r="B70" s="40"/>
+      <c r="C70" s="40"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="45"/>
-      <c r="B71" s="38" t="s">
+      <c r="A71" s="41"/>
+      <c r="B71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="38" t="s">
+      <c r="C71" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="45"/>
-      <c r="B72" s="38" t="s">
+      <c r="A72" s="41"/>
+      <c r="B72" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C72" s="38" t="s">
+      <c r="C72" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="45"/>
-      <c r="B73" s="38" t="s">
+      <c r="A73" s="41"/>
+      <c r="B73" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="38" t="s">
+      <c r="C73" s="34" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="45"/>
-      <c r="B74" s="38" t="s">
+      <c r="A74" s="41"/>
+      <c r="B74" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C74" s="38" t="s">
+      <c r="C74" s="34" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="58" t="s">
+      <c r="A75" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="58"/>
-      <c r="C75" s="58"/>
+      <c r="B75" s="54"/>
+      <c r="C75" s="54"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="46"/>
-      <c r="B76" s="39" t="s">
+      <c r="A76" s="42"/>
+      <c r="B76" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C76" s="38" t="s">
+      <c r="C76" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="47" t="s">
+      <c r="A77" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B77" s="47"/>
-      <c r="C77" s="47"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="43"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="46"/>
-      <c r="B78" s="38" t="s">
+      <c r="A78" s="42"/>
+      <c r="B78" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="38" t="s">
+      <c r="C78" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="46"/>
-      <c r="B79" s="38" t="s">
+      <c r="A79" s="42"/>
+      <c r="B79" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C79" s="38" t="s">
+      <c r="C79" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="46"/>
-      <c r="B80" s="38" t="s">
+      <c r="A80" s="42"/>
+      <c r="B80" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C80" s="38" t="s">
+      <c r="C80" s="34" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="46"/>
-      <c r="B81" s="38" t="s">
+      <c r="A81" s="42"/>
+      <c r="B81" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C81" s="38" t="s">
+      <c r="C81" s="34" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="46"/>
-      <c r="B82" s="38" t="s">
+      <c r="A82" s="42"/>
+      <c r="B82" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C82" s="38"/>
+      <c r="C82" s="34"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="46"/>
-      <c r="B83" s="57" t="s">
+      <c r="A83" s="42"/>
+      <c r="B83" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="C83" s="38" t="s">
+      <c r="C83" s="34" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="46"/>
-      <c r="B84" s="57" t="s">
+      <c r="A84" s="42"/>
+      <c r="B84" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="C84" s="38" t="s">
+      <c r="C84" s="34" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="46"/>
-      <c r="B85" s="57" t="s">
+      <c r="A85" s="42"/>
+      <c r="B85" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="C85" s="38" t="s">
+      <c r="C85" s="34" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="46"/>
-      <c r="B86" s="57" t="s">
+      <c r="A86" s="42"/>
+      <c r="B86" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="C86" s="38" t="s">
+      <c r="C86" s="34" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="46"/>
-      <c r="B87" s="57" t="s">
+      <c r="A87" s="42"/>
+      <c r="B87" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="C87" s="38" t="s">
+      <c r="C87" s="34" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="46"/>
-      <c r="B88" s="57" t="s">
+      <c r="A88" s="42"/>
+      <c r="B88" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="C88" s="38" t="s">
+      <c r="C88" s="34" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="46"/>
-      <c r="B89" s="57" t="s">
+      <c r="A89" s="42"/>
+      <c r="B89" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="C89" s="38" t="s">
+      <c r="C89" s="34" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A90" s="46"/>
-      <c r="B90" s="57" t="s">
+      <c r="A90" s="42"/>
+      <c r="B90" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="C90" s="38" t="s">
+      <c r="C90" s="34" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A91" s="46"/>
-      <c r="B91" s="57" t="s">
+      <c r="A91" s="42"/>
+      <c r="B91" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="C91" s="38" t="s">
+      <c r="C91" s="34" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="60" t="s">
+      <c r="A92" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="B92" s="60"/>
-      <c r="C92" s="60"/>
+      <c r="B92" s="56"/>
+      <c r="C92" s="56"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="9"/>
-      <c r="B93" s="8" t="s">
+      <c r="A93" s="8"/>
+      <c r="B93" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C93" s="63" t="s">
+      <c r="C93" s="59" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A94" s="9"/>
-      <c r="B94" s="8" t="s">
+      <c r="A94" s="8"/>
+      <c r="B94" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C94" s="63" t="s">
+      <c r="C94" s="59" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="50"/>
-      <c r="B95" s="51"/>
-      <c r="C95" s="51"/>
+      <c r="A95" s="46"/>
+      <c r="B95" s="47"/>
+      <c r="C95" s="47"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="50"/>
-      <c r="B96" s="51"/>
-      <c r="C96" s="51"/>
+      <c r="A96" s="46"/>
+      <c r="B96" s="47"/>
+      <c r="C96" s="47"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="50"/>
-      <c r="B97" s="51"/>
-      <c r="C97" s="51"/>
+      <c r="A97" s="46"/>
+      <c r="B97" s="47"/>
+      <c r="C97" s="47"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="52" t="s">
+      <c r="A98" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B98" s="53"/>
-      <c r="C98" s="54"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="50"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="44" t="s">
+      <c r="A99" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B99" s="44"/>
-      <c r="C99" s="44"/>
+      <c r="B99" s="40"/>
+      <c r="C99" s="40"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="45"/>
-      <c r="B100" s="38" t="s">
+      <c r="A100" s="41"/>
+      <c r="B100" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C100" s="38" t="s">
+      <c r="C100" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="45"/>
-      <c r="B101" s="38" t="s">
+      <c r="A101" s="41"/>
+      <c r="B101" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C101" s="38" t="s">
+      <c r="C101" s="34" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="45"/>
-      <c r="B102" s="38" t="s">
+      <c r="A102" s="41"/>
+      <c r="B102" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C102" s="38" t="s">
+      <c r="C102" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="45"/>
-      <c r="B103" s="38" t="s">
+      <c r="A103" s="41"/>
+      <c r="B103" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C103" s="38" t="s">
+      <c r="C103" s="34" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="45"/>
-      <c r="B104" s="38" t="s">
+      <c r="A104" s="41"/>
+      <c r="B104" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C104" s="38" t="s">
+      <c r="C104" s="34" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A105" s="45"/>
-      <c r="B105" s="38" t="s">
+      <c r="A105" s="41"/>
+      <c r="B105" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C105" s="38" t="s">
+      <c r="C105" s="34" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="58" t="s">
+      <c r="A106" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="B106" s="58"/>
-      <c r="C106" s="58"/>
+      <c r="B106" s="54"/>
+      <c r="C106" s="54"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="46"/>
-      <c r="B107" s="39" t="s">
+      <c r="A107" s="42"/>
+      <c r="B107" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C107" s="38" t="s">
+      <c r="C107" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="47" t="s">
+      <c r="A108" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B108" s="47"/>
-      <c r="C108" s="47"/>
+      <c r="B108" s="43"/>
+      <c r="C108" s="43"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="45"/>
-      <c r="B109" s="38" t="s">
+      <c r="A109" s="41"/>
+      <c r="B109" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C109" s="38" t="s">
+      <c r="C109" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="45"/>
-      <c r="B110" s="38" t="s">
+      <c r="A110" s="41"/>
+      <c r="B110" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C110" s="38" t="s">
+      <c r="C110" s="34" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="45"/>
-      <c r="B111" s="38" t="s">
+      <c r="A111" s="41"/>
+      <c r="B111" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C111" s="38" t="s">
+      <c r="C111" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="45"/>
-      <c r="B112" s="38" t="s">
+      <c r="A112" s="41"/>
+      <c r="B112" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C112" s="38" t="s">
+      <c r="C112" s="34" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="113" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="45"/>
-      <c r="B113" s="38" t="s">
+      <c r="A113" s="41"/>
+      <c r="B113" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C113" s="38" t="s">
+      <c r="C113" s="34" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="45"/>
-      <c r="B114" s="57" t="s">
+      <c r="A114" s="41"/>
+      <c r="B114" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="C114" s="38" t="s">
+      <c r="C114" s="34" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="45"/>
-      <c r="B115" s="38" t="s">
+      <c r="A115" s="41"/>
+      <c r="B115" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C115" s="38" t="s">
+      <c r="C115" s="34" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="45"/>
-      <c r="B116" s="57" t="s">
+      <c r="A116" s="41"/>
+      <c r="B116" s="53" t="s">
         <v>171</v>
       </c>
-      <c r="C116" s="38" t="s">
+      <c r="C116" s="34" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="45"/>
-      <c r="B117" s="38" t="s">
+      <c r="A117" s="41"/>
+      <c r="B117" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C117" s="38" t="s">
+      <c r="C117" s="34" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="60" t="s">
+      <c r="A118" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="B118" s="60"/>
-      <c r="C118" s="60"/>
+      <c r="B118" s="56"/>
+      <c r="C118" s="56"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="9"/>
-      <c r="B119" s="9" t="s">
+      <c r="A119" s="8"/>
+      <c r="B119" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C119" s="61" t="s">
+      <c r="C119" s="57" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="55"/>
-      <c r="B120" s="56"/>
-      <c r="C120" s="56"/>
+      <c r="A120" s="51"/>
+      <c r="B120" s="52"/>
+      <c r="C120" s="52"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="52" t="s">
+      <c r="A123" s="48" t="s">
         <v>558</v>
       </c>
-      <c r="B123" s="53"/>
-      <c r="C123" s="59"/>
+      <c r="B123" s="49"/>
+      <c r="C123" s="55"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="44" t="s">
+      <c r="A124" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B124" s="44"/>
-      <c r="C124" s="44"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="45"/>
-      <c r="B125" s="38" t="s">
+      <c r="A125" s="41"/>
+      <c r="B125" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C125" s="38" t="s">
+      <c r="C125" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="45"/>
-      <c r="B126" s="38" t="s">
+      <c r="A126" s="41"/>
+      <c r="B126" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C126" s="38" t="s">
+      <c r="C126" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="45"/>
-      <c r="B127" s="38" t="s">
+      <c r="A127" s="41"/>
+      <c r="B127" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C127" s="38" t="s">
+      <c r="C127" s="34" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="45"/>
-      <c r="B128" s="38" t="s">
+      <c r="A128" s="41"/>
+      <c r="B128" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C128" s="38" t="s">
+      <c r="C128" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="58" t="s">
+      <c r="A129" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="B129" s="58"/>
-      <c r="C129" s="58"/>
+      <c r="B129" s="54"/>
+      <c r="C129" s="54"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="46"/>
-      <c r="B130" s="39" t="s">
+      <c r="A130" s="42"/>
+      <c r="B130" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C130" s="38" t="s">
+      <c r="C130" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="47" t="s">
+      <c r="A131" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B131" s="47"/>
-      <c r="C131" s="47"/>
+      <c r="B131" s="43"/>
+      <c r="C131" s="43"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="45"/>
-      <c r="B132" s="38" t="s">
+      <c r="A132" s="41"/>
+      <c r="B132" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C132" s="38" t="s">
+      <c r="C132" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="45"/>
-      <c r="B133" s="38" t="s">
+      <c r="A133" s="41"/>
+      <c r="B133" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C133" s="38" t="s">
+      <c r="C133" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="46"/>
-      <c r="B134" s="38" t="s">
+      <c r="A134" s="42"/>
+      <c r="B134" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C134" s="38" t="s">
+      <c r="C134" s="34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="46"/>
-      <c r="B135" s="38" t="s">
+      <c r="A135" s="42"/>
+      <c r="B135" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C135" s="38" t="s">
+      <c r="C135" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A136" s="46"/>
-      <c r="B136" s="38" t="s">
+      <c r="A136" s="42"/>
+      <c r="B136" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C136" s="38" t="s">
+      <c r="C136" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="46"/>
-      <c r="B137" s="57" t="s">
+      <c r="A137" s="42"/>
+      <c r="B137" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="C137" s="38" t="s">
+      <c r="C137" s="34" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="46"/>
-      <c r="B138" s="57" t="s">
+      <c r="A138" s="42"/>
+      <c r="B138" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="C138" s="38" t="s">
+      <c r="C138" s="34" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="46"/>
-      <c r="B139" s="57" t="s">
+      <c r="A139" s="42"/>
+      <c r="B139" s="53" t="s">
         <v>183</v>
       </c>
-      <c r="C139" s="38" t="s">
+      <c r="C139" s="34" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="46"/>
-      <c r="B140" s="57" t="s">
+      <c r="A140" s="42"/>
+      <c r="B140" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="C140" s="38" t="s">
+      <c r="C140" s="34" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="46"/>
-      <c r="B141" s="57" t="s">
+      <c r="A141" s="42"/>
+      <c r="B141" s="53" t="s">
         <v>181</v>
       </c>
-      <c r="C141" s="38" t="s">
+      <c r="C141" s="34" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" s="46"/>
-      <c r="B142" s="57" t="s">
+      <c r="A142" s="42"/>
+      <c r="B142" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="C142" s="38" t="s">
+      <c r="C142" s="34" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="46"/>
-      <c r="B143" s="57" t="s">
+      <c r="A143" s="42"/>
+      <c r="B143" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="C143" s="38" t="s">
+      <c r="C143" s="34" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" s="46"/>
-      <c r="B144" s="57" t="s">
+      <c r="A144" s="42"/>
+      <c r="B144" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="C144" s="38" t="s">
+      <c r="C144" s="34" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="46"/>
-      <c r="B145" s="57" t="s">
+      <c r="A145" s="42"/>
+      <c r="B145" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="C145" s="38" t="s">
+      <c r="C145" s="34" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="46"/>
-      <c r="B146" s="57" t="s">
+      <c r="A146" s="42"/>
+      <c r="B146" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="C146" s="38" t="s">
+      <c r="C146" s="34" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="46"/>
-      <c r="B147" s="57" t="s">
+      <c r="A147" s="42"/>
+      <c r="B147" s="53" t="s">
         <v>189</v>
       </c>
-      <c r="C147" s="38" t="s">
+      <c r="C147" s="34" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="46"/>
-      <c r="B148" s="57" t="s">
+      <c r="A148" s="42"/>
+      <c r="B148" s="53" t="s">
         <v>190</v>
       </c>
-      <c r="C148" s="38" t="s">
+      <c r="C148" s="34" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="60" t="s">
+      <c r="A149" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="B149" s="60"/>
-      <c r="C149" s="60"/>
+      <c r="B149" s="56"/>
+      <c r="C149" s="56"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="9"/>
-      <c r="B150" s="9" t="s">
+      <c r="A150" s="8"/>
+      <c r="B150" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C150" s="61" t="s">
+      <c r="C150" s="57" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="50"/>
-      <c r="B151" s="51"/>
-      <c r="C151" s="51"/>
+      <c r="A151" s="46"/>
+      <c r="B151" s="47"/>
+      <c r="C151" s="47"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="50"/>
-      <c r="B152" s="51"/>
-      <c r="C152" s="51"/>
+      <c r="A152" s="46"/>
+      <c r="B152" s="47"/>
+      <c r="C152" s="47"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="50"/>
-      <c r="B153" s="51"/>
-      <c r="C153" s="51"/>
+      <c r="A153" s="46"/>
+      <c r="B153" s="47"/>
+      <c r="C153" s="47"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="52" t="s">
+      <c r="A154" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B154" s="53"/>
-      <c r="C154" s="54"/>
+      <c r="B154" s="49"/>
+      <c r="C154" s="50"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="44" t="s">
+      <c r="A155" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B155" s="44"/>
-      <c r="C155" s="44"/>
+      <c r="B155" s="40"/>
+      <c r="C155" s="40"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" s="45"/>
-      <c r="B156" s="38" t="s">
+      <c r="A156" s="41"/>
+      <c r="B156" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C156" s="38" t="s">
+      <c r="C156" s="34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="45"/>
-      <c r="B157" s="38" t="s">
+      <c r="A157" s="41"/>
+      <c r="B157" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C157" s="38" t="s">
+      <c r="C157" s="34" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" s="45"/>
-      <c r="B158" s="38" t="s">
+      <c r="A158" s="41"/>
+      <c r="B158" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C158" s="38" t="s">
+      <c r="C158" s="34" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="58" t="s">
+      <c r="A159" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="B159" s="58"/>
-      <c r="C159" s="58"/>
+      <c r="B159" s="54"/>
+      <c r="C159" s="54"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="46"/>
-      <c r="B160" s="39" t="s">
+      <c r="A160" s="42"/>
+      <c r="B160" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C160" s="38" t="s">
+      <c r="C160" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="47" t="s">
+      <c r="A161" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B161" s="47"/>
-      <c r="C161" s="47"/>
+      <c r="B161" s="43"/>
+      <c r="C161" s="43"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="46"/>
-      <c r="B162" s="38" t="s">
+      <c r="A162" s="42"/>
+      <c r="B162" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C162" s="38" t="s">
+      <c r="C162" s="34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="46"/>
-      <c r="B163" s="38" t="s">
+      <c r="A163" s="42"/>
+      <c r="B163" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C163" s="38"/>
+      <c r="C163" s="34"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" s="46"/>
-      <c r="B164" s="57" t="s">
+      <c r="A164" s="42"/>
+      <c r="B164" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="C164" s="38" t="s">
+      <c r="C164" s="34" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" s="46"/>
-      <c r="B165" s="57" t="s">
+      <c r="A165" s="42"/>
+      <c r="B165" s="53" t="s">
         <v>229</v>
       </c>
-      <c r="C165" s="38" t="s">
+      <c r="C165" s="34" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" s="46"/>
-      <c r="B166" s="57" t="s">
+      <c r="A166" s="42"/>
+      <c r="B166" s="53" t="s">
         <v>230</v>
       </c>
-      <c r="C166" s="38" t="s">
+      <c r="C166" s="34" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" s="46"/>
-      <c r="B167" s="57" t="s">
+      <c r="A167" s="42"/>
+      <c r="B167" s="53" t="s">
         <v>236</v>
       </c>
-      <c r="C167" s="38" t="s">
+      <c r="C167" s="34" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" s="46"/>
-      <c r="B168" s="57" t="s">
+      <c r="A168" s="42"/>
+      <c r="B168" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="C168" s="38" t="s">
+      <c r="C168" s="34" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" s="46"/>
-      <c r="B169" s="57" t="s">
+      <c r="A169" s="42"/>
+      <c r="B169" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="C169" s="38" t="s">
+      <c r="C169" s="34" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" s="46"/>
-      <c r="B170" s="57" t="s">
+      <c r="A170" s="42"/>
+      <c r="B170" s="53" t="s">
         <v>232</v>
       </c>
-      <c r="C170" s="38" t="s">
+      <c r="C170" s="34" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" s="46"/>
-      <c r="B171" s="57" t="s">
+      <c r="A171" s="42"/>
+      <c r="B171" s="53" t="s">
         <v>233</v>
       </c>
-      <c r="C171" s="38" t="s">
+      <c r="C171" s="34" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A172" s="46"/>
-      <c r="B172" s="57" t="s">
+      <c r="A172" s="42"/>
+      <c r="B172" s="53" t="s">
         <v>234</v>
       </c>
-      <c r="C172" s="38" t="s">
+      <c r="C172" s="34" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A173" s="46"/>
-      <c r="B173" s="57" t="s">
+      <c r="A173" s="42"/>
+      <c r="B173" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="C173" s="38" t="s">
+      <c r="C173" s="34" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" s="46"/>
-      <c r="B174" s="38" t="s">
+      <c r="A174" s="42"/>
+      <c r="B174" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C174" s="38" t="s">
+      <c r="C174" s="34" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" s="46"/>
-      <c r="B175" s="38" t="s">
+      <c r="A175" s="42"/>
+      <c r="B175" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C175" s="38" t="s">
+      <c r="C175" s="34" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" s="46"/>
-      <c r="B176" s="38" t="s">
+      <c r="A176" s="42"/>
+      <c r="B176" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="C176" s="38" t="s">
+      <c r="C176" s="34" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" s="46"/>
-      <c r="B177" s="57" t="s">
+      <c r="A177" s="42"/>
+      <c r="B177" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="C177" s="38" t="s">
+      <c r="C177" s="34" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A178" s="46"/>
-      <c r="B178" s="57" t="s">
+      <c r="A178" s="42"/>
+      <c r="B178" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="C178" s="38" t="s">
+      <c r="C178" s="34" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="46"/>
-      <c r="B179" s="38" t="s">
+      <c r="A179" s="42"/>
+      <c r="B179" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="C179" s="38" t="s">
+      <c r="C179" s="34" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" s="46"/>
-      <c r="B180" s="57" t="s">
+      <c r="A180" s="42"/>
+      <c r="B180" s="53" t="s">
         <v>377</v>
       </c>
-      <c r="C180" s="38" t="s">
+      <c r="C180" s="34" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181" s="46"/>
-      <c r="B181" s="57" t="s">
+      <c r="A181" s="42"/>
+      <c r="B181" s="53" t="s">
         <v>376</v>
       </c>
-      <c r="C181" s="38" t="s">
+      <c r="C181" s="34" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" s="46"/>
-      <c r="B182" s="38" t="s">
+      <c r="A182" s="42"/>
+      <c r="B182" s="34" t="s">
         <v>349</v>
       </c>
-      <c r="C182" s="38" t="s">
+      <c r="C182" s="34" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" s="46"/>
-      <c r="B183" s="38" t="s">
+      <c r="A183" s="42"/>
+      <c r="B183" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="C183" s="38" t="s">
+      <c r="C183" s="34" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A184" s="46"/>
-      <c r="B184" s="38" t="s">
+      <c r="A184" s="42"/>
+      <c r="B184" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="C184" s="38" t="s">
+      <c r="C184" s="34" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" s="60" t="s">
+      <c r="A185" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="B185" s="60"/>
-      <c r="C185" s="60"/>
+      <c r="B185" s="56"/>
+      <c r="C185" s="56"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" s="9"/>
-      <c r="B186" s="9" t="s">
+      <c r="A186" s="8"/>
+      <c r="B186" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C186" s="62" t="s">
+      <c r="C186" s="58" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A190" s="52" t="s">
+      <c r="A190" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="B190" s="53"/>
-      <c r="C190" s="54"/>
+      <c r="B190" s="49"/>
+      <c r="C190" s="50"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" s="44" t="s">
+      <c r="A191" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B191" s="44"/>
-      <c r="C191" s="44"/>
+      <c r="B191" s="40"/>
+      <c r="C191" s="40"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192" s="45"/>
-      <c r="B192" s="38" t="s">
+      <c r="A192" s="41"/>
+      <c r="B192" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="C192" s="38" t="s">
+      <c r="C192" s="34" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="45"/>
-      <c r="B193" s="38" t="s">
+      <c r="A193" s="41"/>
+      <c r="B193" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="C193" s="38" t="s">
+      <c r="C193" s="34" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="45"/>
-      <c r="B194" s="38" t="s">
+      <c r="A194" s="41"/>
+      <c r="B194" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C194" s="38" t="s">
+      <c r="C194" s="34" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="58" t="s">
+      <c r="A195" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="B195" s="58"/>
-      <c r="C195" s="58"/>
+      <c r="B195" s="54"/>
+      <c r="C195" s="54"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="46"/>
-      <c r="B196" s="39" t="s">
+      <c r="A196" s="42"/>
+      <c r="B196" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C196" s="38" t="s">
+      <c r="C196" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="47" t="s">
+      <c r="A197" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B197" s="47"/>
-      <c r="C197" s="47"/>
+      <c r="B197" s="43"/>
+      <c r="C197" s="43"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198" s="46"/>
-      <c r="B198" s="38" t="s">
+      <c r="A198" s="42"/>
+      <c r="B198" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="C198" s="38" t="s">
+      <c r="C198" s="34" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" s="46"/>
-      <c r="B199" s="38" t="s">
+      <c r="A199" s="42"/>
+      <c r="B199" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="C199" s="38" t="s">
+      <c r="C199" s="34" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" s="46"/>
-      <c r="B200" s="38" t="s">
+      <c r="A200" s="42"/>
+      <c r="B200" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C200" s="38" t="s">
+      <c r="C200" s="34" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="60" t="s">
+      <c r="A201" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="B201" s="60"/>
-      <c r="C201" s="60"/>
+      <c r="B201" s="56"/>
+      <c r="C201" s="56"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" s="9"/>
-      <c r="B202" s="9" t="s">
+      <c r="A202" s="8"/>
+      <c r="B202" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C202" s="62" t="s">
+      <c r="C202" s="58" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" s="52" t="s">
+      <c r="A206" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="B206" s="53"/>
-      <c r="C206" s="54"/>
+      <c r="B206" s="49"/>
+      <c r="C206" s="50"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207" s="44" t="s">
+      <c r="A207" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B207" s="44"/>
-      <c r="C207" s="44"/>
+      <c r="B207" s="40"/>
+      <c r="C207" s="40"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A208" s="45"/>
-      <c r="B208" s="38" t="s">
+      <c r="A208" s="41"/>
+      <c r="B208" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="C208" s="38" t="s">
+      <c r="C208" s="34" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A209" s="45"/>
-      <c r="B209" s="38" t="s">
+      <c r="A209" s="41"/>
+      <c r="B209" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="C209" s="38" t="s">
+      <c r="C209" s="34" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A210" s="45"/>
-      <c r="B210" s="38" t="s">
+      <c r="A210" s="41"/>
+      <c r="B210" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="C210" s="38" t="s">
+      <c r="C210" s="34" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211" s="45"/>
-      <c r="B211" s="38" t="s">
+      <c r="A211" s="41"/>
+      <c r="B211" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="C211" s="38" t="s">
+      <c r="C211" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A212" s="58" t="s">
+      <c r="A212" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="B212" s="58"/>
-      <c r="C212" s="58"/>
+      <c r="B212" s="54"/>
+      <c r="C212" s="54"/>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A213" s="46"/>
-      <c r="B213" s="39" t="s">
+      <c r="A213" s="42"/>
+      <c r="B213" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C213" s="38" t="s">
+      <c r="C213" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A214" s="47" t="s">
+      <c r="A214" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B214" s="47"/>
-      <c r="C214" s="47"/>
+      <c r="B214" s="43"/>
+      <c r="C214" s="43"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A215" s="46"/>
-      <c r="B215" s="38" t="s">
+      <c r="A215" s="42"/>
+      <c r="B215" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="C215" s="38" t="s">
+      <c r="C215" s="34" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A216" s="46"/>
-      <c r="B216" s="38" t="s">
+      <c r="A216" s="42"/>
+      <c r="B216" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="C216" s="38" t="s">
+      <c r="C216" s="34" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A217" s="46"/>
-      <c r="B217" s="38" t="s">
+      <c r="A217" s="42"/>
+      <c r="B217" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="C217" s="38" t="s">
+      <c r="C217" s="34" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A218" s="46"/>
-      <c r="B218" s="38" t="s">
+      <c r="A218" s="42"/>
+      <c r="B218" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="C218" s="38" t="s">
+      <c r="C218" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A219" s="60" t="s">
+      <c r="A219" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="B219" s="60"/>
-      <c r="C219" s="60"/>
+      <c r="B219" s="56"/>
+      <c r="C219" s="56"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A220" s="9"/>
-      <c r="B220" s="9" t="s">
+      <c r="A220" s="8"/>
+      <c r="B220" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C220" s="62" t="s">
+      <c r="C220" s="58" t="s">
         <v>258</v>
       </c>
     </row>
@@ -7852,175 +7871,191 @@
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="86.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="86.44140625" style="47" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="22"/>
-      <c r="B1" s="6"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="52"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="84" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="52" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="52">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="52"/>
     </row>
     <row r="6" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="52"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="52" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="52" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="52"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="52"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="52"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="85" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="52" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="83" t="s">
+      <c r="A14" s="79" t="s">
         <v>602</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="52" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="15" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="52"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="52"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="52"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="52"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="52"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="86" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="52" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="52"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="52" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="52"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="52"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="52"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="52"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="52"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="52"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -8072,7 +8107,7 @@
     <col min="19" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="71" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="67" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -8085,16 +8120,16 @@
       <c r="D1" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -8125,28 +8160,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67" t="s">
+    <row r="2" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="63"/>
+      <c r="B2" s="63" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
     </row>
     <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E3" s="2" t="s">
@@ -8302,13 +8337,13 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="65" t="s">
         <v>283</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -8331,13 +8366,13 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="65" t="s">
         <v>325</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="65" t="s">
         <v>283</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -8385,28 +8420,28 @@
         <v>388</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="67" t="s">
+    <row r="12" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="63"/>
+      <c r="B12" s="63" t="s">
         <v>286</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67" t="s">
+      <c r="C12" s="64"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="67"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E13" s="2" t="s">
@@ -8532,28 +8567,28 @@
         <v>431</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
-      <c r="B18" s="67" t="s">
+    <row r="18" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="63"/>
+      <c r="B18" s="63" t="s">
         <v>291</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67" t="s">
+      <c r="C18" s="64"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="67"/>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="67"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -8659,28 +8694,28 @@
         <v>358</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="67" t="s">
+    <row r="23" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="63"/>
+      <c r="B23" s="63" t="s">
         <v>267</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67" t="s">
+      <c r="C23" s="64"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="68"/>
-      <c r="N23" s="68"/>
-      <c r="O23" s="67"/>
-      <c r="P23" s="67"/>
-      <c r="Q23" s="67"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E24" s="2" t="s">
@@ -8729,13 +8764,13 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="D26" s="69" t="s">
+      <c r="D26" s="65" t="s">
         <v>304</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -8755,13 +8790,13 @@
       </c>
     </row>
     <row r="27" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="D27" s="69" t="s">
+      <c r="D27" s="65" t="s">
         <v>304</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -8784,13 +8819,13 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B28" s="69" t="s">
+      <c r="B28" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C28" s="69" t="s">
+      <c r="C28" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="D28" s="69" t="s">
+      <c r="D28" s="65" t="s">
         <v>304</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -8943,13 +8978,13 @@
       </c>
     </row>
     <row r="34" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="C34" s="69" t="s">
+      <c r="C34" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="D34" s="69" t="s">
+      <c r="D34" s="65" t="s">
         <v>312</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -9021,13 +9056,13 @@
       </c>
     </row>
     <row r="37" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="69" t="s">
+      <c r="B37" s="65" t="s">
         <v>315</v>
       </c>
-      <c r="C37" s="69" t="s">
+      <c r="C37" s="65" t="s">
         <v>402</v>
       </c>
-      <c r="D37" s="69" t="s">
+      <c r="D37" s="65" t="s">
         <v>318</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -9046,15 +9081,15 @@
         <v>508</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="69" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="65" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
-      <c r="B38" s="69" t="s">
+      <c r="B38" s="65" t="s">
         <v>315</v>
       </c>
-      <c r="C38" s="69" t="s">
+      <c r="C38" s="65" t="s">
         <v>402</v>
       </c>
-      <c r="D38" s="69" t="s">
+      <c r="D38" s="65" t="s">
         <v>318</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -9083,15 +9118,15 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" s="69" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="65" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="65" t="s">
         <v>315</v>
       </c>
-      <c r="C39" s="69" t="s">
+      <c r="C39" s="65" t="s">
         <v>402</v>
       </c>
-      <c r="D39" s="69" t="s">
+      <c r="D39" s="65" t="s">
         <v>318</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -9121,29 +9156,29 @@
       <c r="Q39" s="2"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" s="67"/>
-      <c r="B40" s="67" t="s">
+      <c r="A40" s="63"/>
+      <c r="B40" s="63" t="s">
         <v>319</v>
       </c>
-      <c r="C40" s="68"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67" t="s">
+      <c r="C40" s="64"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="68"/>
-      <c r="K40" s="67"/>
-      <c r="L40" s="68"/>
-      <c r="M40" s="68"/>
-      <c r="N40" s="68"/>
-      <c r="O40" s="67"/>
-      <c r="P40" s="67"/>
-      <c r="Q40" s="67"/>
-    </row>
-    <row r="41" spans="1:17" s="69" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F40" s="63"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="64"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="64"/>
+      <c r="N40" s="64"/>
+      <c r="O40" s="63"/>
+      <c r="P40" s="63"/>
+      <c r="Q40" s="63"/>
+    </row>
+    <row r="41" spans="1:17" s="65" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
         <v>303</v>
@@ -9178,12 +9213,12 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
-      <c r="B42" s="69" t="s">
+      <c r="B42" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C42" s="69" t="s">
+      <c r="C42" s="65" t="s">
         <v>334</v>
       </c>
       <c r="D42" s="2"/>
@@ -9213,12 +9248,12 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
-      <c r="B43" s="69" t="s">
+      <c r="B43" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C43" s="69" t="s">
+      <c r="C43" s="65" t="s">
         <v>334</v>
       </c>
       <c r="D43" s="2"/>
@@ -9247,27 +9282,27 @@
       <c r="Q43" s="2"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" s="67"/>
-      <c r="B44" s="67" t="s">
+      <c r="A44" s="63"/>
+      <c r="B44" s="63" t="s">
         <v>276</v>
       </c>
-      <c r="C44" s="68"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="67" t="s">
+      <c r="C44" s="64"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="67"/>
-      <c r="G44" s="67"/>
-      <c r="H44" s="67"/>
-      <c r="I44" s="67"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="67"/>
-      <c r="L44" s="68"/>
-      <c r="M44" s="68"/>
-      <c r="N44" s="68"/>
-      <c r="O44" s="67"/>
-      <c r="P44" s="67"/>
-      <c r="Q44" s="67"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="64"/>
+      <c r="N44" s="64"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="63"/>
     </row>
     <row r="45" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E45" s="2" t="s">
@@ -9316,13 +9351,13 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B47" s="69" t="s">
+      <c r="B47" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C47" s="69" t="s">
+      <c r="C47" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="D47" s="69" t="s">
+      <c r="D47" s="65" t="s">
         <v>304</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -9345,13 +9380,13 @@
       </c>
     </row>
     <row r="48" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B48" s="69" t="s">
+      <c r="B48" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C48" s="69" t="s">
+      <c r="C48" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="D48" s="69" t="s">
+      <c r="D48" s="65" t="s">
         <v>304</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -9374,13 +9409,13 @@
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C49" s="69" t="s">
+      <c r="C49" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="D49" s="69" t="s">
+      <c r="D49" s="65" t="s">
         <v>304</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -9478,27 +9513,27 @@
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" s="67"/>
-      <c r="B53" s="67" t="s">
+      <c r="A53" s="63"/>
+      <c r="B53" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="C53" s="68"/>
-      <c r="D53" s="67"/>
-      <c r="E53" s="67" t="s">
+      <c r="C53" s="64"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="F53" s="67"/>
-      <c r="G53" s="67"/>
-      <c r="H53" s="67"/>
-      <c r="I53" s="67"/>
-      <c r="J53" s="68"/>
-      <c r="K53" s="67"/>
-      <c r="L53" s="68"/>
-      <c r="M53" s="68"/>
-      <c r="N53" s="68"/>
-      <c r="O53" s="67"/>
-      <c r="P53" s="67"/>
-      <c r="Q53" s="67"/>
+      <c r="F53" s="63"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="63"/>
+      <c r="J53" s="64"/>
+      <c r="K53" s="63"/>
+      <c r="L53" s="64"/>
+      <c r="M53" s="64"/>
+      <c r="N53" s="64"/>
+      <c r="O53" s="63"/>
+      <c r="P53" s="63"/>
+      <c r="Q53" s="63"/>
     </row>
     <row r="54" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
@@ -9576,7 +9611,7 @@
     <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="71" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="67" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -9589,16 +9624,16 @@
       <c r="D1" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -9624,10 +9659,10 @@
       <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>411</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -9641,23 +9676,23 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="65" t="s">
         <v>385</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69" t="s">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65" t="s">
         <v>384</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>412</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>413</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -9786,13 +9821,13 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="65" t="s">
         <v>327</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -9835,13 +9870,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="65" t="s">
         <v>302</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -9904,11 +9939,11 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69" t="s">
+      <c r="C14" s="65"/>
+      <c r="D14" s="65" t="s">
         <v>300</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -9966,7 +10001,7 @@
     <col min="2" max="2" width="29.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.77734375" style="2" customWidth="1"/>
-    <col min="5" max="6" width="11.77734375" style="21" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" style="20" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" style="2" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" hidden="1" customWidth="1"/>
@@ -9974,56 +10009,56 @@
     <col min="11" max="11" width="23.88671875" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
     <col min="13" max="13" width="30.6640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.77734375" style="21" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" style="21" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" style="20" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" style="20" customWidth="1"/>
     <col min="16" max="16" width="43.6640625" style="2" customWidth="1"/>
     <col min="17" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="71" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:16" s="67" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>559</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>569</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>562</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>572</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="18" t="s">
         <v>573</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -10031,26 +10066,26 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="65"/>
-      <c r="B2" s="67" t="s">
+      <c r="A2" s="61"/>
+      <c r="B2" s="63" t="s">
         <v>285</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="67" t="s">
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="65"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="61"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -10375,26 +10410,26 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="65"/>
-      <c r="B17" s="67" t="s">
+      <c r="A17" s="61"/>
+      <c r="B17" s="63" t="s">
         <v>341</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="67" t="s">
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="65"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="61"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
@@ -10420,11 +10455,11 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69" t="s">
+      <c r="C19" s="65"/>
+      <c r="D19" s="65" t="s">
         <v>303</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -10444,11 +10479,11 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="69" t="s">
+      <c r="B20" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69" t="s">
+      <c r="C20" s="65"/>
+      <c r="D20" s="65" t="s">
         <v>303</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -10584,11 +10619,11 @@
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69" t="s">
+      <c r="C26" s="65"/>
+      <c r="D26" s="65" t="s">
         <v>311</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -10657,11 +10692,11 @@
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B29" s="69" t="s">
+      <c r="B29" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69" t="s">
+      <c r="C29" s="65"/>
+      <c r="D29" s="65" t="s">
         <v>315</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -10681,11 +10716,11 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="69" t="s">
+      <c r="B30" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69" t="s">
+      <c r="C30" s="65"/>
+      <c r="D30" s="65" t="s">
         <v>315</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -10705,26 +10740,26 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
-      <c r="B31" s="67" t="s">
+      <c r="A31" s="61"/>
+      <c r="B31" s="63" t="s">
         <v>342</v>
       </c>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="67" t="s">
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
-      <c r="M31" s="65"/>
-      <c r="N31" s="70"/>
-      <c r="O31" s="70"/>
-      <c r="P31" s="65"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="61"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="61"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
@@ -10750,11 +10785,11 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B33" s="69" t="s">
+      <c r="B33" s="65" t="s">
         <v>319</v>
       </c>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69" t="s">
+      <c r="C33" s="65"/>
+      <c r="D33" s="65" t="s">
         <v>303</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -10774,26 +10809,26 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
-      <c r="B34" s="67" t="s">
+      <c r="A34" s="61"/>
+      <c r="B34" s="63" t="s">
         <v>343</v>
       </c>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="67" t="s">
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
-      <c r="L34" s="65"/>
-      <c r="M34" s="65"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="65"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="61"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
@@ -10865,11 +10900,11 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B38" s="69" t="s">
+      <c r="B38" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69" t="s">
+      <c r="C38" s="65"/>
+      <c r="D38" s="65" t="s">
         <v>303</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -10889,11 +10924,11 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69" t="s">
+      <c r="C39" s="65"/>
+      <c r="D39" s="65" t="s">
         <v>303</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -10982,26 +11017,26 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A43" s="65"/>
-      <c r="B43" s="67" t="s">
+      <c r="A43" s="61"/>
+      <c r="B43" s="63" t="s">
         <v>389</v>
       </c>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="67" t="s">
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H43" s="65"/>
-      <c r="I43" s="65"/>
-      <c r="J43" s="65"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="65"/>
-      <c r="M43" s="65"/>
-      <c r="N43" s="70"/>
-      <c r="O43" s="70"/>
-      <c r="P43" s="65"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+      <c r="L43" s="61"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="66"/>
+      <c r="O43" s="66"/>
+      <c r="P43" s="61"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
@@ -11126,178 +11161,178 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="21" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="21" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="21" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" style="21" customWidth="1"/>
-    <col min="10" max="10" width="32.88671875" style="21" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" style="21" customWidth="1"/>
-    <col min="12" max="12" width="40.6640625" style="21" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" style="21" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="21"/>
+    <col min="1" max="1" width="11.6640625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="20" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="20" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="20" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" style="20" customWidth="1"/>
+    <col min="10" max="10" width="32.88671875" style="20" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="40.6640625" style="20" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" style="20" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="72" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:13" s="68" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="73" t="s">
         <v>559</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="74" t="s">
         <v>560</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="74" t="s">
         <v>553</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="74" t="s">
         <v>561</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="75" t="s">
         <v>550</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="79" t="s">
+      <c r="H1" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="80" t="s">
+      <c r="I1" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="77" t="s">
         <v>562</v>
       </c>
-      <c r="K1" s="82" t="s">
+      <c r="K1" s="78" t="s">
         <v>563</v>
       </c>
-      <c r="L1" s="82" t="s">
+      <c r="L1" s="78" t="s">
         <v>556</v>
       </c>
-      <c r="M1" s="82" t="s">
+      <c r="M1" s="78" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75" t="s">
+      <c r="A2" s="71"/>
+      <c r="B2" s="71" t="s">
         <v>385</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="71" t="s">
         <v>337</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75" t="s">
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71" t="s">
         <v>351</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J2" s="71" t="s">
         <v>411</v>
       </c>
-      <c r="K2" s="75" t="s">
+      <c r="K2" s="71" t="s">
         <v>337</v>
       </c>
-      <c r="L2" s="75" t="s">
+      <c r="L2" s="71" t="s">
         <v>410</v>
       </c>
-      <c r="M2" s="75"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="75"/>
-      <c r="B3" s="75" t="s">
+      <c r="A3" s="71"/>
+      <c r="B3" s="71" t="s">
         <v>385</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="71" t="s">
         <v>338</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75" t="s">
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75" t="s">
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71" t="s">
         <v>351</v>
       </c>
-      <c r="J3" s="75" t="s">
+      <c r="J3" s="71" t="s">
         <v>411</v>
       </c>
-      <c r="K3" s="75" t="s">
+      <c r="K3" s="71" t="s">
         <v>338</v>
       </c>
-      <c r="L3" s="75" t="s">
+      <c r="L3" s="71" t="s">
         <v>536</v>
       </c>
-      <c r="M3" s="75"/>
+      <c r="M3" s="71"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75" t="s">
+      <c r="A4" s="71"/>
+      <c r="B4" s="71" t="s">
         <v>385</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="71" t="s">
         <v>335</v>
       </c>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75" t="s">
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71" t="s">
         <v>351</v>
       </c>
-      <c r="J4" s="75" t="s">
+      <c r="J4" s="71" t="s">
         <v>411</v>
       </c>
-      <c r="K4" s="75" t="s">
+      <c r="K4" s="71" t="s">
         <v>335</v>
       </c>
-      <c r="L4" s="75" t="s">
+      <c r="L4" s="71" t="s">
         <v>408</v>
       </c>
-      <c r="M4" s="75"/>
+      <c r="M4" s="71"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="71" t="s">
         <v>385</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="71" t="s">
         <v>336</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75" t="s">
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75" t="s">
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71" t="s">
         <v>351</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="71" t="s">
         <v>411</v>
       </c>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="71" t="s">
         <v>336</v>
       </c>
-      <c r="L5" s="75" t="s">
+      <c r="L5" s="71" t="s">
         <v>409</v>
       </c>
-      <c r="M5" s="75"/>
+      <c r="M5" s="71"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -11336,55 +11371,55 @@
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.77734375" style="73" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" style="73" customWidth="1"/>
+    <col min="2" max="2" width="55.77734375" style="69" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" style="69" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
     <col min="5" max="6" width="29.109375" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="73" customWidth="1"/>
-    <col min="8" max="8" width="13" style="73" customWidth="1"/>
-    <col min="9" max="9" width="55.77734375" style="73" customWidth="1"/>
-    <col min="10" max="10" width="35.77734375" style="73" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="73" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="69" customWidth="1"/>
+    <col min="8" max="8" width="13" style="69" customWidth="1"/>
+    <col min="9" max="9" width="55.77734375" style="69" customWidth="1"/>
+    <col min="10" max="10" width="35.77734375" style="69" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="69" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="23.5546875" style="2" customWidth="1"/>
     <col min="14" max="14" width="35.44140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" style="74" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" style="70" customWidth="1"/>
     <col min="16" max="16" width="9.109375" style="2" customWidth="1"/>
     <col min="17" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="71" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:15" s="67" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>574</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>553</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>575</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>576</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>556</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>348</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -11396,7 +11431,7 @@
       <c r="N1" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="62" t="s">
         <v>580</v>
       </c>
     </row>
@@ -11404,16 +11439,16 @@
       <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="69" t="s">
         <v>351</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="69" t="s">
         <v>403</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="69" t="s">
         <v>404</v>
       </c>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="69" t="s">
         <v>407</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -11425,7 +11460,7 @@
       <c r="N2" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="O2" s="74" t="s">
+      <c r="O2" s="70" t="s">
         <v>406</v>
       </c>
     </row>
@@ -11482,37 +11517,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>599</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>598</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>594</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>597</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>595</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>596</v>
       </c>
     </row>

</xml_diff>